<commit_message>
updated zone definition and drawings
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JLeckie\Documents\GitHub\Arena\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B390EEAD-157E-4948-9AB5-FDF2BE0F5ADD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4133989-872E-49A6-8F03-A4A1E10CB65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10230" yWindow="-15" windowWidth="10275" windowHeight="10950" activeTab="1" xr2:uid="{8EA56093-14A8-493C-A0C9-93774F80DC09}"/>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="10245" windowHeight="10950" xr2:uid="{2FAC1D7F-10DE-46D7-B2B3-D27D8DDA8493}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2FAC1D7F-10DE-46D7-B2B3-D27D8DDA8493}"/>
   </bookViews>
   <sheets>
-    <sheet name="Player" sheetId="1" r:id="rId1"/>
-    <sheet name="Characters" sheetId="4" r:id="rId2"/>
-    <sheet name="Skills &amp; Spells" sheetId="3" r:id="rId3"/>
-    <sheet name="Unused" sheetId="2" r:id="rId4"/>
+    <sheet name="Main" sheetId="5" r:id="rId1"/>
+    <sheet name="Player" sheetId="1" r:id="rId2"/>
+    <sheet name="Characters" sheetId="4" r:id="rId3"/>
+    <sheet name="Skills &amp; Spells" sheetId="3" r:id="rId4"/>
+    <sheet name="Unused" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="377">
   <si>
     <t>Attribute</t>
   </si>
@@ -853,13 +853,331 @@
   </si>
   <si>
     <t>fortitude: int</t>
+  </si>
+  <si>
+    <t>import</t>
+  </si>
+  <si>
+    <t>menu</t>
+  </si>
+  <si>
+    <t>characters</t>
+  </si>
+  <si>
+    <t>player</t>
+  </si>
+  <si>
+    <t>area</t>
+  </si>
+  <si>
+    <t>schedules</t>
+  </si>
+  <si>
+    <t>colors</t>
+  </si>
+  <si>
+    <t>random</t>
+  </si>
+  <si>
+    <t>os.system</t>
+  </si>
+  <si>
+    <t>Items.items</t>
+  </si>
+  <si>
+    <t>items.init('Items/Items.csv')</t>
+  </si>
+  <si>
+    <t>colors.init()</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>height</t>
+  </si>
+  <si>
+    <t>walls</t>
+  </si>
+  <si>
+    <t>[list]</t>
+  </si>
+  <si>
+    <t>(2, 2), (2, height - 3), (width - 3, 2), (width - 3, height - 3)</t>
+  </si>
+  <si>
+    <t>zone_arena</t>
+  </si>
+  <si>
+    <t>area.Area(width, height, walls)</t>
+  </si>
+  <si>
+    <t>arena_spawn</t>
+  </si>
+  <si>
+    <t>(x, y) not in walls</t>
+  </si>
+  <si>
+    <t>room</t>
+  </si>
+  <si>
+    <t>random.choice(arena_spawn)</t>
+  </si>
+  <si>
+    <t>characters.Fighter(room[0], room[1], 'A Fighter')</t>
+  </si>
+  <si>
+    <t>def __main__():</t>
+  </si>
+  <si>
+    <t>menu.start_menu()</t>
+  </si>
+  <si>
+    <t>schedules.mob_timer.start()</t>
+  </si>
+  <si>
+    <t>y == 0</t>
+  </si>
+  <si>
+    <t>x == 0</t>
+  </si>
+  <si>
+    <t>x == width - 1</t>
+  </si>
+  <si>
+    <t>y == height - 1</t>
+  </si>
+  <si>
+    <t>while True:</t>
+  </si>
+  <si>
+    <t>system('cls')</t>
+  </si>
+  <si>
+    <t>print('\n\n\n')</t>
+  </si>
+  <si>
+    <t>if menu.menu(arena):</t>
+  </si>
+  <si>
+    <t>print("Quitting...")</t>
+  </si>
+  <si>
+    <t>schedules.mob_timer.stop()</t>
+  </si>
+  <si>
+    <t>exit()</t>
+  </si>
+  <si>
+    <t>__main__()</t>
+  </si>
+  <si>
+    <t>characters.Character.all_characters</t>
+  </si>
+  <si>
+    <t>player.main_player</t>
+  </si>
+  <si>
+    <t>player.main_player)</t>
+  </si>
+  <si>
+    <t>arena.show(</t>
+  </si>
+  <si>
+    <t>area.show_creatures(</t>
+  </si>
+  <si>
+    <t>player.main_player.loc_x</t>
+  </si>
+  <si>
+    <t>player.main_player.loc_y</t>
+  </si>
+  <si>
+    <t>characters.Character.all_characters)</t>
+  </si>
+  <si>
+    <t>MAIN.py</t>
+  </si>
+  <si>
+    <t>MENU.py</t>
+  </si>
+  <si>
+    <t>player.new_player</t>
+  </si>
+  <si>
+    <t>player.load_player</t>
+  </si>
+  <si>
+    <t>player.save_player</t>
+  </si>
+  <si>
+    <t>colors.Effect</t>
+  </si>
+  <si>
+    <t>colors.Fore</t>
+  </si>
+  <si>
+    <t>colors.Back</t>
+  </si>
+  <si>
+    <t>~~~~~ Pre-Game Menu ~~~~~</t>
+  </si>
+  <si>
+    <t>def start_menu():</t>
+  </si>
+  <si>
+    <t>print('Welcome…')</t>
+  </si>
+  <si>
+    <t>print('by Joel Leckie')</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>New Game</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Load Game</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Instructions</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>Settings</t>
+  </si>
+  <si>
+    <t>Q</t>
+  </si>
+  <si>
+    <t>Quit</t>
+  </si>
+  <si>
+    <t>cmd</t>
+  </si>
+  <si>
+    <t>input('Your command?')</t>
+  </si>
+  <si>
+    <t>cmd == 'n'</t>
+  </si>
+  <si>
+    <t>if new_game(): break</t>
+  </si>
+  <si>
+    <t>cmd == 'l'</t>
+  </si>
+  <si>
+    <t>if load_game(): break</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>cmd == 's'</t>
+  </si>
+  <si>
+    <t>cmd == 'q'</t>
+  </si>
+  <si>
+    <t>n = new = new game</t>
+  </si>
+  <si>
+    <t>l = load = load game</t>
+  </si>
+  <si>
+    <t>i = instruction = instructions</t>
+  </si>
+  <si>
+    <t>s = set = setting = settings</t>
+  </si>
+  <si>
+    <t>q = quit</t>
+  </si>
+  <si>
+    <t>cmd == 'i'</t>
+  </si>
+  <si>
+    <t>def new_game():</t>
+  </si>
+  <si>
+    <t>def load_game():</t>
+  </si>
+  <si>
+    <t>def instructions():</t>
+  </si>
+  <si>
+    <t>def settings():</t>
+  </si>
+  <si>
+    <t>print('Type RETURN to go back to the main menu')</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>input('Enter your name…')</t>
+  </si>
+  <si>
+    <t>name == 'RETURN'</t>
+  </si>
+  <si>
+    <t>return False</t>
+  </si>
+  <si>
+    <t>print('error…')</t>
+  </si>
+  <si>
+    <t>name[0].upper() + name[1:].lower()</t>
+  </si>
+  <si>
+    <t>break</t>
+  </si>
+  <si>
+    <t>new_player(name)</t>
+  </si>
+  <si>
+    <t>return True</t>
+  </si>
+  <si>
+    <t>name.isdigit() or not name.isalpha()</t>
+  </si>
+  <si>
+    <t>load_player(name)</t>
+  </si>
+  <si>
+    <t>else</t>
+  </si>
+  <si>
+    <t>~~~~~ In-Game Menu ~~~~~</t>
+  </si>
+  <si>
+    <t>def menu(place):</t>
+  </si>
+  <si>
+    <t>exits</t>
+  </si>
+  <si>
+    <t>place.exits(main_player.loc_x, main_player.loc_y)</t>
+  </si>
+  <si>
+    <t>print('Available exits…')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -875,8 +1193,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -925,8 +1250,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1012,26 +1373,183 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1041,12 +1559,12 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1360,13 +1878,1225 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F86FC45-D7D5-4164-8A37-790C1A972BE9}">
+  <dimension ref="A1:AO52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="H40" workbookViewId="0">
+      <selection activeCell="Z53" sqref="Z53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="4.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="4.28515625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A1" s="39" t="s">
+        <v>318</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="39"/>
+      <c r="G1" s="39"/>
+      <c r="H1" s="39"/>
+      <c r="I1" s="39"/>
+      <c r="J1" s="39"/>
+      <c r="K1" s="39"/>
+      <c r="L1" s="39"/>
+      <c r="M1" s="39"/>
+      <c r="N1" s="39"/>
+      <c r="O1" s="39"/>
+      <c r="P1" s="39"/>
+      <c r="Q1" s="39"/>
+      <c r="R1" s="39"/>
+      <c r="S1" s="39"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="39" t="s">
+        <v>319</v>
+      </c>
+      <c r="W1" s="39"/>
+      <c r="X1" s="39"/>
+      <c r="Y1" s="39"/>
+      <c r="Z1" s="39"/>
+      <c r="AA1" s="39"/>
+      <c r="AB1" s="39"/>
+      <c r="AC1" s="39"/>
+      <c r="AD1" s="39"/>
+      <c r="AE1" s="39"/>
+      <c r="AF1" s="39"/>
+      <c r="AG1" s="39"/>
+      <c r="AH1" s="39"/>
+      <c r="AI1" s="39"/>
+      <c r="AJ1" s="39"/>
+      <c r="AK1" s="39"/>
+      <c r="AL1" s="39"/>
+      <c r="AM1" s="39"/>
+      <c r="AN1" s="39"/>
+      <c r="AO1" s="39"/>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="U2" s="12"/>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A3" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="B3" s="40"/>
+      <c r="C3" s="37" t="s">
+        <v>272</v>
+      </c>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37" t="s">
+        <v>273</v>
+      </c>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37" t="s">
+        <v>274</v>
+      </c>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37" t="s">
+        <v>276</v>
+      </c>
+      <c r="M3" s="37"/>
+      <c r="N3" s="37"/>
+      <c r="O3" s="37" t="s">
+        <v>277</v>
+      </c>
+      <c r="P3" s="37"/>
+      <c r="Q3" s="37" t="s">
+        <v>280</v>
+      </c>
+      <c r="R3" s="37"/>
+      <c r="S3" s="37"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="40" t="s">
+        <v>271</v>
+      </c>
+      <c r="W3" s="40"/>
+      <c r="X3" s="37" t="s">
+        <v>275</v>
+      </c>
+      <c r="Y3" s="41"/>
+      <c r="Z3" s="37" t="s">
+        <v>320</v>
+      </c>
+      <c r="AA3" s="37"/>
+      <c r="AB3" s="37"/>
+      <c r="AC3" s="37"/>
+      <c r="AD3" s="37" t="s">
+        <v>321</v>
+      </c>
+      <c r="AE3" s="37"/>
+      <c r="AF3" s="37"/>
+      <c r="AG3" s="37"/>
+      <c r="AH3" s="37" t="s">
+        <v>322</v>
+      </c>
+      <c r="AI3" s="37"/>
+      <c r="AJ3" s="37"/>
+      <c r="AK3" s="37"/>
+      <c r="AL3" s="37" t="s">
+        <v>311</v>
+      </c>
+      <c r="AM3" s="37"/>
+      <c r="AN3" s="37"/>
+      <c r="AO3" s="37"/>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="C4" s="37" t="s">
+        <v>278</v>
+      </c>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37" t="s">
+        <v>279</v>
+      </c>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+      <c r="N4" s="14"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="U4" s="12"/>
+      <c r="X4" s="37" t="s">
+        <v>279</v>
+      </c>
+      <c r="Y4" s="37"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="37" t="s">
+        <v>323</v>
+      </c>
+      <c r="AB4" s="37"/>
+      <c r="AC4" s="38"/>
+      <c r="AD4" s="37" t="s">
+        <v>324</v>
+      </c>
+      <c r="AE4" s="37"/>
+      <c r="AF4" s="38"/>
+      <c r="AG4" s="37" t="s">
+        <v>325</v>
+      </c>
+      <c r="AH4" s="37"/>
+      <c r="AI4" s="38"/>
+      <c r="AJ4" s="14"/>
+      <c r="AK4" s="14"/>
+      <c r="AL4" s="14"/>
+      <c r="AM4" s="14"/>
+      <c r="AN4" s="14"/>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="U5" s="12"/>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="39" t="s">
+        <v>326</v>
+      </c>
+      <c r="W6" s="39"/>
+      <c r="X6" s="39"/>
+      <c r="Y6" s="39"/>
+      <c r="Z6" s="39"/>
+      <c r="AA6" s="39"/>
+      <c r="AB6" s="39"/>
+      <c r="AC6" s="39"/>
+      <c r="AD6" s="39"/>
+      <c r="AE6" s="39"/>
+      <c r="AF6" s="39"/>
+      <c r="AG6" s="39"/>
+      <c r="AH6" s="39"/>
+      <c r="AI6" s="39"/>
+      <c r="AJ6" s="39"/>
+      <c r="AK6" s="39"/>
+      <c r="AL6" s="39"/>
+      <c r="AM6" s="39"/>
+      <c r="AN6" s="39"/>
+      <c r="AO6" s="39"/>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="U7" s="12"/>
+      <c r="V7" s="26" t="s">
+        <v>327</v>
+      </c>
+      <c r="W7" s="26"/>
+      <c r="X7" s="26"/>
+      <c r="Y7" s="26"/>
+      <c r="Z7" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="AA7" s="20"/>
+      <c r="AB7" s="20"/>
+      <c r="AC7" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="AD7" s="35"/>
+      <c r="AE7" s="35"/>
+      <c r="AF7" s="35"/>
+      <c r="AG7" s="35"/>
+      <c r="AH7" s="36"/>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="U8" s="12"/>
+      <c r="AC8" s="34" t="s">
+        <v>328</v>
+      </c>
+      <c r="AD8" s="35"/>
+      <c r="AE8" s="35"/>
+      <c r="AF8" s="35"/>
+      <c r="AG8" s="35"/>
+      <c r="AH8" s="36"/>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A9" s="24" t="s">
+        <v>283</v>
+      </c>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24" t="s">
+        <v>284</v>
+      </c>
+      <c r="D9" s="24"/>
+      <c r="E9" s="11">
+        <v>10</v>
+      </c>
+      <c r="U9" s="12"/>
+      <c r="AC9" s="34" t="s">
+        <v>329</v>
+      </c>
+      <c r="AD9" s="35"/>
+      <c r="AE9" s="35"/>
+      <c r="AF9" s="35"/>
+      <c r="AG9" s="35"/>
+      <c r="AH9" s="36"/>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A10" s="24" t="s">
+        <v>285</v>
+      </c>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="E10" s="24"/>
+      <c r="F10" s="25" t="s">
+        <v>287</v>
+      </c>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
+      <c r="J10" s="25"/>
+      <c r="K10" s="25"/>
+      <c r="L10" s="25"/>
+      <c r="M10" s="25"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="U10" s="12"/>
+      <c r="AC10" s="15" t="s">
+        <v>330</v>
+      </c>
+      <c r="AD10" s="30" t="s">
+        <v>331</v>
+      </c>
+      <c r="AE10" s="31"/>
+      <c r="AF10" s="31"/>
+      <c r="AG10" s="32"/>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="F11" s="43" t="s">
+        <v>299</v>
+      </c>
+      <c r="G11" s="43"/>
+      <c r="H11" s="43" t="s">
+        <v>300</v>
+      </c>
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="43" t="s">
+        <v>298</v>
+      </c>
+      <c r="M11" s="43"/>
+      <c r="N11" s="43" t="s">
+        <v>301</v>
+      </c>
+      <c r="O11" s="43"/>
+      <c r="P11" s="43"/>
+      <c r="Q11" s="43"/>
+      <c r="U11" s="12"/>
+      <c r="AC11" s="15" t="s">
+        <v>332</v>
+      </c>
+      <c r="AD11" s="28" t="s">
+        <v>333</v>
+      </c>
+      <c r="AE11" s="28"/>
+      <c r="AF11" s="28"/>
+      <c r="AG11" s="28"/>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="U12" s="12"/>
+      <c r="AC12" s="15" t="s">
+        <v>334</v>
+      </c>
+      <c r="AD12" s="28" t="s">
+        <v>335</v>
+      </c>
+      <c r="AE12" s="28"/>
+      <c r="AF12" s="28"/>
+      <c r="AG12" s="28"/>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="25" t="s">
+        <v>289</v>
+      </c>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
+      <c r="I13" s="25"/>
+      <c r="J13" s="25"/>
+      <c r="U13" s="12"/>
+      <c r="AC13" s="15" t="s">
+        <v>336</v>
+      </c>
+      <c r="AD13" s="28" t="s">
+        <v>337</v>
+      </c>
+      <c r="AE13" s="28"/>
+      <c r="AF13" s="28"/>
+      <c r="AG13" s="28"/>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A14" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="E14" s="24"/>
+      <c r="F14" s="25" t="s">
+        <v>291</v>
+      </c>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="25"/>
+      <c r="U14" s="12"/>
+      <c r="AC14" s="16" t="s">
+        <v>338</v>
+      </c>
+      <c r="AD14" s="29" t="s">
+        <v>339</v>
+      </c>
+      <c r="AE14" s="29"/>
+      <c r="AF14" s="29"/>
+      <c r="AG14" s="29"/>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="25" t="s">
+        <v>293</v>
+      </c>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="25"/>
+      <c r="U15" s="12"/>
+      <c r="AC15" s="24" t="s">
+        <v>340</v>
+      </c>
+      <c r="AD15" s="24"/>
+      <c r="AE15" s="25" t="s">
+        <v>341</v>
+      </c>
+      <c r="AF15" s="25"/>
+      <c r="AG15" s="25"/>
+      <c r="AH15" s="25"/>
+      <c r="AI15" s="25"/>
+      <c r="AJ15" s="25"/>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A16" s="17" t="s">
+        <v>294</v>
+      </c>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="U16" s="12"/>
+      <c r="V16" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="W16" s="33"/>
+      <c r="X16" s="33"/>
+      <c r="Y16" s="33"/>
+      <c r="Z16" s="33"/>
+      <c r="AA16" s="33"/>
+      <c r="AC16" s="23" t="s">
+        <v>342</v>
+      </c>
+      <c r="AD16" s="23"/>
+      <c r="AE16" s="23"/>
+      <c r="AF16" s="20" t="s">
+        <v>343</v>
+      </c>
+      <c r="AG16" s="20"/>
+      <c r="AH16" s="20"/>
+      <c r="AI16" s="20"/>
+      <c r="AJ16" s="20"/>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U17" s="12"/>
+      <c r="V17" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="W17" s="33"/>
+      <c r="X17" s="33"/>
+      <c r="Y17" s="33"/>
+      <c r="Z17" s="33"/>
+      <c r="AA17" s="33"/>
+      <c r="AC17" s="23" t="s">
+        <v>344</v>
+      </c>
+      <c r="AD17" s="23"/>
+      <c r="AE17" s="23"/>
+      <c r="AF17" s="20" t="s">
+        <v>345</v>
+      </c>
+      <c r="AG17" s="20"/>
+      <c r="AH17" s="20"/>
+      <c r="AI17" s="20"/>
+      <c r="AJ17" s="20"/>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A18" s="26" t="s">
+        <v>295</v>
+      </c>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="17" t="s">
+        <v>296</v>
+      </c>
+      <c r="F18" s="17"/>
+      <c r="G18" s="17"/>
+      <c r="H18" s="17"/>
+      <c r="I18" s="17"/>
+      <c r="J18" s="17"/>
+      <c r="K18" s="17"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="33" t="s">
+        <v>351</v>
+      </c>
+      <c r="W18" s="33"/>
+      <c r="X18" s="33"/>
+      <c r="Y18" s="33"/>
+      <c r="Z18" s="33"/>
+      <c r="AA18" s="33"/>
+      <c r="AC18" s="23" t="s">
+        <v>354</v>
+      </c>
+      <c r="AD18" s="23"/>
+      <c r="AE18" s="23"/>
+      <c r="AF18" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="AG18" s="20"/>
+      <c r="AH18" s="20"/>
+      <c r="AI18" s="20"/>
+      <c r="AJ18" s="20"/>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="E19" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="U19" s="12"/>
+      <c r="V19" s="33" t="s">
+        <v>352</v>
+      </c>
+      <c r="W19" s="33"/>
+      <c r="X19" s="33"/>
+      <c r="Y19" s="33"/>
+      <c r="Z19" s="33"/>
+      <c r="AA19" s="33"/>
+      <c r="AC19" s="23" t="s">
+        <v>347</v>
+      </c>
+      <c r="AD19" s="23"/>
+      <c r="AE19" s="23"/>
+      <c r="AF19" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="AG19" s="20"/>
+      <c r="AH19" s="20"/>
+      <c r="AI19" s="20"/>
+      <c r="AJ19" s="20"/>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="E20" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="F20" s="20"/>
+      <c r="G20" s="20"/>
+      <c r="H20" s="34" t="s">
+        <v>303</v>
+      </c>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="36"/>
+      <c r="U20" s="12"/>
+      <c r="V20" s="33" t="s">
+        <v>353</v>
+      </c>
+      <c r="W20" s="33"/>
+      <c r="X20" s="33"/>
+      <c r="Y20" s="33"/>
+      <c r="Z20" s="33"/>
+      <c r="AA20" s="33"/>
+      <c r="AC20" s="23" t="s">
+        <v>348</v>
+      </c>
+      <c r="AD20" s="23"/>
+      <c r="AE20" s="23"/>
+      <c r="AF20" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="AG20" s="20"/>
+      <c r="AH20" s="20"/>
+      <c r="AI20" s="20"/>
+      <c r="AJ20" s="20"/>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="H21" s="34" t="s">
+        <v>304</v>
+      </c>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
+      <c r="M21" s="36"/>
+      <c r="U21" s="12"/>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="H22" s="34" t="s">
+        <v>313</v>
+      </c>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="36"/>
+      <c r="U22" s="12"/>
+      <c r="V22" s="26" t="s">
+        <v>355</v>
+      </c>
+      <c r="W22" s="26"/>
+      <c r="X22" s="26"/>
+      <c r="Y22" s="26"/>
+      <c r="Z22" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="AA22" s="17"/>
+      <c r="AB22" s="17"/>
+      <c r="AC22" s="17"/>
+      <c r="AD22" s="17"/>
+      <c r="AE22" s="17"/>
+      <c r="AF22" s="17"/>
+      <c r="AG22" s="17"/>
+      <c r="AH22" s="17"/>
+      <c r="AI22" s="17"/>
+      <c r="AJ22" s="17"/>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="K23" s="17" t="s">
+        <v>310</v>
+      </c>
+      <c r="L23" s="17"/>
+      <c r="M23" s="17"/>
+      <c r="N23" s="17"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="17"/>
+      <c r="Q23" s="17"/>
+      <c r="R23" s="17"/>
+      <c r="U23" s="12"/>
+      <c r="Z23" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="AA23" s="20"/>
+      <c r="AB23" s="20"/>
+      <c r="AC23" s="27" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD23" s="27"/>
+      <c r="AE23" s="25" t="s">
+        <v>361</v>
+      </c>
+      <c r="AF23" s="25"/>
+      <c r="AG23" s="25"/>
+      <c r="AH23" s="25"/>
+      <c r="AI23" s="25"/>
+      <c r="AJ23" s="25"/>
+    </row>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="K24" s="42" t="s">
+        <v>312</v>
+      </c>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="17"/>
+      <c r="Q24" s="17"/>
+      <c r="R24" s="17"/>
+      <c r="U24" s="12"/>
+      <c r="AC24" s="21" t="s">
+        <v>362</v>
+      </c>
+      <c r="AD24" s="21"/>
+      <c r="AE24" s="21"/>
+      <c r="AF24" s="21"/>
+      <c r="AG24" s="22" t="s">
+        <v>363</v>
+      </c>
+      <c r="AH24" s="22"/>
+      <c r="AI24" s="22"/>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="H25" s="17" t="s">
+        <v>314</v>
+      </c>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="U25" s="12"/>
+      <c r="AC25" s="23" t="s">
+        <v>369</v>
+      </c>
+      <c r="AD25" s="23"/>
+      <c r="AE25" s="23"/>
+      <c r="AF25" s="23"/>
+      <c r="AG25" s="23"/>
+      <c r="AH25" s="23"/>
+      <c r="AI25" s="23"/>
+      <c r="AJ25" s="23"/>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="K26" s="17" t="s">
+        <v>315</v>
+      </c>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
+      <c r="U26" s="12"/>
+      <c r="AG26" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="AH26" s="17"/>
+      <c r="AI26" s="17"/>
+      <c r="AJ26" s="17"/>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="K27" s="17" t="s">
+        <v>316</v>
+      </c>
+      <c r="L27" s="17"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="17"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="17"/>
+      <c r="Q27" s="17"/>
+      <c r="R27" s="17"/>
+      <c r="U27" s="12"/>
+      <c r="AC27" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD27" s="24"/>
+      <c r="AE27" s="25" t="s">
+        <v>365</v>
+      </c>
+      <c r="AF27" s="25"/>
+      <c r="AG27" s="25"/>
+      <c r="AH27" s="25"/>
+      <c r="AI27" s="25"/>
+      <c r="AJ27" s="25"/>
+      <c r="AK27" s="25"/>
+      <c r="AL27" s="25"/>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="K28" s="17" t="s">
+        <v>317</v>
+      </c>
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="U28" s="12"/>
+      <c r="AC28" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="AD28" s="17"/>
+      <c r="AE28" s="18"/>
+      <c r="AF28" s="18"/>
+      <c r="AG28" s="18"/>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="H29" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="17" t="s">
+        <v>306</v>
+      </c>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="U29" s="12"/>
+      <c r="AC29" s="19" t="s">
+        <v>366</v>
+      </c>
+      <c r="AD29" s="19"/>
+      <c r="AE29" s="19"/>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="M30" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="17"/>
+      <c r="Q30" s="17"/>
+      <c r="R30" s="17"/>
+      <c r="U30" s="12"/>
+      <c r="Z30" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="AA30" s="17"/>
+      <c r="AB30" s="17"/>
+      <c r="AC30" s="17"/>
+      <c r="AD30" s="17"/>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="M31" s="17" t="s">
+        <v>308</v>
+      </c>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="U31" s="12"/>
+      <c r="Z31" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="AA31" s="19"/>
+      <c r="AB31" s="19"/>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U32" s="12"/>
+    </row>
+    <row r="33" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>309</v>
+      </c>
+      <c r="B33" s="17"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="U33" s="12"/>
+      <c r="V33" s="26" t="s">
+        <v>356</v>
+      </c>
+      <c r="W33" s="26"/>
+      <c r="X33" s="26"/>
+      <c r="Y33" s="26"/>
+      <c r="Z33" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="AA33" s="17"/>
+      <c r="AB33" s="17"/>
+      <c r="AC33" s="17"/>
+      <c r="AD33" s="17"/>
+      <c r="AE33" s="17"/>
+      <c r="AF33" s="17"/>
+      <c r="AG33" s="17"/>
+      <c r="AH33" s="17"/>
+      <c r="AI33" s="17"/>
+      <c r="AJ33" s="17"/>
+    </row>
+    <row r="34" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U34" s="12"/>
+      <c r="Z34" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="AA34" s="20"/>
+      <c r="AB34" s="20"/>
+      <c r="AC34" s="27" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD34" s="27"/>
+      <c r="AE34" s="25" t="s">
+        <v>361</v>
+      </c>
+      <c r="AF34" s="25"/>
+      <c r="AG34" s="25"/>
+      <c r="AH34" s="25"/>
+      <c r="AI34" s="25"/>
+      <c r="AJ34" s="25"/>
+    </row>
+    <row r="35" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U35" s="12"/>
+      <c r="AC35" s="21" t="s">
+        <v>362</v>
+      </c>
+      <c r="AD35" s="21"/>
+      <c r="AE35" s="21"/>
+      <c r="AF35" s="21"/>
+      <c r="AG35" s="22" t="s">
+        <v>363</v>
+      </c>
+      <c r="AH35" s="22"/>
+      <c r="AI35" s="22"/>
+    </row>
+    <row r="36" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U36" s="12"/>
+      <c r="AC36" s="23" t="s">
+        <v>369</v>
+      </c>
+      <c r="AD36" s="23"/>
+      <c r="AE36" s="23"/>
+      <c r="AF36" s="23"/>
+      <c r="AG36" s="23"/>
+      <c r="AH36" s="23"/>
+      <c r="AI36" s="23"/>
+      <c r="AJ36" s="23"/>
+    </row>
+    <row r="37" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U37" s="12"/>
+      <c r="AG37" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="AH37" s="17"/>
+      <c r="AI37" s="17"/>
+      <c r="AJ37" s="17"/>
+    </row>
+    <row r="38" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U38" s="12"/>
+      <c r="AC38" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="AD38" s="24"/>
+      <c r="AE38" s="25" t="s">
+        <v>365</v>
+      </c>
+      <c r="AF38" s="25"/>
+      <c r="AG38" s="25"/>
+      <c r="AH38" s="25"/>
+      <c r="AI38" s="25"/>
+      <c r="AJ38" s="25"/>
+      <c r="AK38" s="25"/>
+      <c r="AL38" s="25"/>
+    </row>
+    <row r="39" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U39" s="12"/>
+      <c r="AC39" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="AD39" s="17"/>
+      <c r="AE39" s="17"/>
+      <c r="AF39" s="17"/>
+      <c r="AG39" s="17"/>
+      <c r="AH39" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="AI39" s="17"/>
+      <c r="AJ39" s="18"/>
+      <c r="AK39" s="18"/>
+      <c r="AL39" s="18"/>
+    </row>
+    <row r="40" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U40" s="12"/>
+      <c r="AH40" s="19" t="s">
+        <v>366</v>
+      </c>
+      <c r="AI40" s="19"/>
+      <c r="AJ40" s="19"/>
+    </row>
+    <row r="41" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U41" s="12"/>
+      <c r="AC41" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="AD41" s="20"/>
+      <c r="AE41" s="20" t="s">
+        <v>363</v>
+      </c>
+      <c r="AF41" s="20"/>
+      <c r="AG41" s="20"/>
+    </row>
+    <row r="42" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U42" s="12"/>
+      <c r="Z42" s="20" t="s">
+        <v>368</v>
+      </c>
+      <c r="AA42" s="20"/>
+      <c r="AB42" s="20"/>
+    </row>
+    <row r="43" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U43" s="12"/>
+    </row>
+    <row r="44" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U44" s="12"/>
+    </row>
+    <row r="45" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U45" s="12"/>
+      <c r="V45" s="26" t="s">
+        <v>357</v>
+      </c>
+      <c r="W45" s="26"/>
+      <c r="X45" s="26"/>
+      <c r="Y45" s="26"/>
+      <c r="Z45" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="AA45" s="20"/>
+    </row>
+    <row r="46" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U46" s="12"/>
+    </row>
+    <row r="47" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U47" s="12"/>
+    </row>
+    <row r="48" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="U48" s="12"/>
+      <c r="V48" s="26" t="s">
+        <v>358</v>
+      </c>
+      <c r="W48" s="26"/>
+      <c r="X48" s="26"/>
+      <c r="Y48" s="26"/>
+      <c r="Z48" s="20" t="s">
+        <v>346</v>
+      </c>
+      <c r="AA48" s="20"/>
+    </row>
+    <row r="49" spans="21:41" x14ac:dyDescent="0.25">
+      <c r="U49" s="12"/>
+    </row>
+    <row r="50" spans="21:41" x14ac:dyDescent="0.25">
+      <c r="U50" s="12"/>
+      <c r="V50" s="39" t="s">
+        <v>372</v>
+      </c>
+      <c r="W50" s="39"/>
+      <c r="X50" s="39"/>
+      <c r="Y50" s="39"/>
+      <c r="Z50" s="39"/>
+      <c r="AA50" s="39"/>
+      <c r="AB50" s="39"/>
+      <c r="AC50" s="39"/>
+      <c r="AD50" s="39"/>
+      <c r="AE50" s="39"/>
+      <c r="AF50" s="39"/>
+      <c r="AG50" s="39"/>
+      <c r="AH50" s="39"/>
+      <c r="AI50" s="39"/>
+      <c r="AJ50" s="39"/>
+      <c r="AK50" s="39"/>
+      <c r="AL50" s="39"/>
+      <c r="AM50" s="39"/>
+      <c r="AN50" s="39"/>
+      <c r="AO50" s="39"/>
+    </row>
+    <row r="51" spans="21:41" x14ac:dyDescent="0.25">
+      <c r="V51" s="10" t="s">
+        <v>373</v>
+      </c>
+      <c r="Z51" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="AB51" s="10" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="52" spans="21:41" x14ac:dyDescent="0.25">
+      <c r="Z52" s="10" t="s">
+        <v>376</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="124">
+    <mergeCell ref="V50:AO50"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="Q3:S3"/>
+    <mergeCell ref="A6:H6"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:G4"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="A7:H7"/>
+    <mergeCell ref="H22:M22"/>
+    <mergeCell ref="E20:G20"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="H11:K11"/>
+    <mergeCell ref="D13:J13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:J14"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:Q10"/>
+    <mergeCell ref="V1:AO1"/>
+    <mergeCell ref="M31:R31"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="X4:Z4"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="AD3:AG3"/>
+    <mergeCell ref="AH3:AK3"/>
+    <mergeCell ref="K26:R26"/>
+    <mergeCell ref="K27:R27"/>
+    <mergeCell ref="K28:R28"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="M30:R30"/>
+    <mergeCell ref="M29:R29"/>
+    <mergeCell ref="K23:R23"/>
+    <mergeCell ref="K24:R24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="D15:J15"/>
+    <mergeCell ref="E19:K19"/>
+    <mergeCell ref="E18:K18"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="AC7:AH7"/>
+    <mergeCell ref="Z7:AB7"/>
+    <mergeCell ref="V7:Y7"/>
+    <mergeCell ref="AC8:AH8"/>
+    <mergeCell ref="AC9:AH9"/>
+    <mergeCell ref="AL3:AO3"/>
+    <mergeCell ref="AA4:AC4"/>
+    <mergeCell ref="AD4:AF4"/>
+    <mergeCell ref="AG4:AI4"/>
+    <mergeCell ref="V6:AO6"/>
+    <mergeCell ref="AD11:AG11"/>
+    <mergeCell ref="AD12:AG12"/>
+    <mergeCell ref="AD13:AG13"/>
+    <mergeCell ref="AD14:AG14"/>
+    <mergeCell ref="AD10:AG10"/>
+    <mergeCell ref="V16:AA16"/>
+    <mergeCell ref="V17:AA17"/>
+    <mergeCell ref="V18:AA18"/>
+    <mergeCell ref="V19:AA19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="Z23:AB23"/>
+    <mergeCell ref="Z34:AB34"/>
+    <mergeCell ref="V22:Y22"/>
+    <mergeCell ref="V33:Y33"/>
+    <mergeCell ref="AC23:AD23"/>
+    <mergeCell ref="AC15:AD15"/>
+    <mergeCell ref="AC16:AE16"/>
+    <mergeCell ref="AC17:AE17"/>
+    <mergeCell ref="AC18:AE18"/>
+    <mergeCell ref="AC19:AE19"/>
+    <mergeCell ref="AC20:AE20"/>
+    <mergeCell ref="AE15:AJ15"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="V20:AA20"/>
+    <mergeCell ref="V45:Y45"/>
+    <mergeCell ref="V48:Y48"/>
+    <mergeCell ref="Z45:AA45"/>
+    <mergeCell ref="Z48:AA48"/>
+    <mergeCell ref="Z31:AB31"/>
+    <mergeCell ref="AG24:AI24"/>
+    <mergeCell ref="AE27:AL27"/>
+    <mergeCell ref="AG26:AJ26"/>
+    <mergeCell ref="AC34:AD34"/>
+    <mergeCell ref="AE34:AJ34"/>
+    <mergeCell ref="Z22:AJ22"/>
+    <mergeCell ref="Z33:AJ33"/>
+    <mergeCell ref="Z30:AD30"/>
+    <mergeCell ref="AC29:AE29"/>
+    <mergeCell ref="AC27:AD27"/>
+    <mergeCell ref="AC24:AF24"/>
+    <mergeCell ref="AE23:AJ23"/>
+    <mergeCell ref="AC25:AJ25"/>
+    <mergeCell ref="AC28:AG28"/>
+    <mergeCell ref="AH39:AL39"/>
+    <mergeCell ref="AH40:AJ40"/>
+    <mergeCell ref="Z42:AB42"/>
+    <mergeCell ref="AE41:AG41"/>
+    <mergeCell ref="AC41:AD41"/>
+    <mergeCell ref="AC39:AG39"/>
+    <mergeCell ref="AC35:AF35"/>
+    <mergeCell ref="AG35:AI35"/>
+    <mergeCell ref="AC36:AJ36"/>
+    <mergeCell ref="AG37:AJ37"/>
+    <mergeCell ref="AC38:AD38"/>
+    <mergeCell ref="AE38:AL38"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F31AF466-7B57-4515-9AAA-B8FC02C9F00F}">
   <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
-    </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
       <selection activeCell="A47" sqref="A47:D52"/>
     </sheetView>
   </sheetViews>
@@ -1393,27 +3123,27 @@
       <c r="A1" t="s">
         <v>250</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="I1" s="2"/>
+      <c r="I1" s="44"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="44" t="s">
         <v>201</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
+      <c r="N1" s="44"/>
+      <c r="O1" s="44"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="44" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
       <c r="H2" t="s">
         <v>217</v>
       </c>
@@ -1902,14 +3632,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C445B14-EB09-4409-9C6D-BF1F0176B277}">
   <dimension ref="A1:L55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50:F50"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1928,34 +3657,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="48" t="s">
         <v>216</v>
       </c>
-      <c r="B1" s="12"/>
+      <c r="B1" s="49"/>
       <c r="I1" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="4" t="s">
         <v>265</v>
       </c>
       <c r="I2" t="s">
@@ -1972,19 +3701,19 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="9" t="s">
         <v>270</v>
       </c>
       <c r="I3" t="s">
@@ -1998,10 +3727,10 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>267</v>
       </c>
       <c r="I4" t="s">
@@ -2015,15 +3744,15 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="45" t="s">
         <v>221</v>
       </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="11"/>
+      <c r="B5" s="46"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="47"/>
       <c r="I5" t="s">
         <v>237</v>
       </c>
@@ -2035,7 +3764,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="6" t="s">
         <v>222</v>
       </c>
       <c r="I6" t="s">
@@ -2046,12 +3775,12 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="2" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>224</v>
       </c>
       <c r="I8" t="s">
@@ -2059,7 +3788,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="2" t="s">
         <v>225</v>
       </c>
       <c r="I9" t="s">
@@ -2076,7 +3805,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="2" t="s">
         <v>226</v>
       </c>
       <c r="I10" t="s">
@@ -2090,7 +3819,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B11" t="s">
@@ -2124,7 +3853,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B13" t="s">
@@ -2146,7 +3875,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>252</v>
       </c>
       <c r="B15" t="s">
@@ -2177,7 +3906,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="I17" t="s">
@@ -2191,7 +3920,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
       <c r="I18" t="s">
@@ -2205,7 +3934,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="I19" t="s">
@@ -2219,7 +3948,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
+      <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I20" t="s">
@@ -2230,12 +3959,12 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
         <v>179</v>
       </c>
       <c r="B22" t="s">
@@ -2260,7 +3989,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
         <v>25</v>
       </c>
       <c r="B24" t="s">
@@ -2329,7 +4058,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="A30" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B30" t="s">
@@ -2392,68 +4121,68 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="49" t="s">
         <v>232</v>
       </c>
-      <c r="B38" s="12"/>
+      <c r="B38" s="49"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="E39" s="5" t="s">
+      <c r="E39" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="F39" s="5" t="s">
+      <c r="F39" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="G39" s="4" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="C40" s="15" t="s">
+      <c r="C40" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E40" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F40" s="9" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
+      <c r="A41" s="2" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="2" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
+      <c r="A43" s="2" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="8" t="s">
         <v>191</v>
       </c>
       <c r="B44" t="s">
@@ -2461,7 +4190,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="8" t="s">
         <v>192</v>
       </c>
       <c r="B46" t="s">
@@ -2469,68 +4198,68 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="B48" s="6"/>
+      <c r="B48" s="48"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="E49" s="5" t="s">
+      <c r="E49" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="F49" s="5" t="s">
+      <c r="F49" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="G49" s="5" t="s">
+      <c r="G49" s="4" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="9" t="s">
         <v>230</v>
       </c>
-      <c r="C50" s="15" t="s">
+      <c r="C50" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="E50" s="15" t="s">
+      <c r="E50" s="9" t="s">
         <v>269</v>
       </c>
-      <c r="F50" s="15" t="s">
+      <c r="F50" s="9" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+      <c r="A51" s="2" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+      <c r="A52" s="2" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+      <c r="A53" s="2" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="2" t="s">
         <v>254</v>
       </c>
       <c r="B54" t="s">
@@ -2538,7 +4267,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="14" t="s">
+      <c r="A55" s="8" t="s">
         <v>253</v>
       </c>
     </row>
@@ -2554,14 +4283,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD03DC4-F366-4B40-852C-8A0CB60D942C}">
   <dimension ref="A2:J52"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3064,14 +4790,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3BA5F0-F4D6-42DF-955B-2C6E884E8104}">
   <dimension ref="A1:A8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Added alternate color names, updated player starting stats
</commit_message>
<xml_diff>
--- a/Planning.xlsx
+++ b/Planning.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JLeckie\Documents\GitHub\Arena\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4133989-872E-49A6-8F03-A4A1E10CB65F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2785B000-7ACC-44C1-A9E9-6D1B4E6AB922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2FAC1D7F-10DE-46D7-B2B3-D27D8DDA8493}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{2FAC1D7F-10DE-46D7-B2B3-D27D8DDA8493}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="5" r:id="rId1"/>
     <sheet name="Player" sheetId="1" r:id="rId2"/>
     <sheet name="Characters" sheetId="4" r:id="rId3"/>
     <sheet name="Skills &amp; Spells" sheetId="3" r:id="rId4"/>
-    <sheet name="Unused" sheetId="2" r:id="rId5"/>
+    <sheet name="Gathering &amp; Crafting" sheetId="6" r:id="rId5"/>
+    <sheet name="Creatures" sheetId="7" r:id="rId6"/>
+    <sheet name="City" sheetId="8" r:id="rId7"/>
+    <sheet name="Unused" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="565">
   <si>
     <t>Attribute</t>
   </si>
@@ -1171,6 +1174,570 @@
   </si>
   <si>
     <t>print('Available exits…')</t>
+  </si>
+  <si>
+    <t>Herbalism</t>
+  </si>
+  <si>
+    <t>Copper</t>
+  </si>
+  <si>
+    <t>Smithing</t>
+  </si>
+  <si>
+    <t>Helm</t>
+  </si>
+  <si>
+    <t>Helmet</t>
+  </si>
+  <si>
+    <t>Bracers</t>
+  </si>
+  <si>
+    <t>Gauntlets</t>
+  </si>
+  <si>
+    <t>Greaves</t>
+  </si>
+  <si>
+    <t>Boots</t>
+  </si>
+  <si>
+    <t>Chainmail</t>
+  </si>
+  <si>
+    <t>Scalemail</t>
+  </si>
+  <si>
+    <t>Suit of Plates</t>
+  </si>
+  <si>
+    <t>Platemail</t>
+  </si>
+  <si>
+    <t>Tailoring</t>
+  </si>
+  <si>
+    <t>Cotton</t>
+  </si>
+  <si>
+    <t>Hemp</t>
+  </si>
+  <si>
+    <t>Silk</t>
+  </si>
+  <si>
+    <t>Cap</t>
+  </si>
+  <si>
+    <t>Hat</t>
+  </si>
+  <si>
+    <t>Gloves</t>
+  </si>
+  <si>
+    <t>Sandals</t>
+  </si>
+  <si>
+    <t>Hand Wraps</t>
+  </si>
+  <si>
+    <t>Bandana</t>
+  </si>
+  <si>
+    <t>Foot Wraps</t>
+  </si>
+  <si>
+    <t>Shirt</t>
+  </si>
+  <si>
+    <t>Tunic</t>
+  </si>
+  <si>
+    <t>Robes</t>
+  </si>
+  <si>
+    <t>Birch</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Bow</t>
+  </si>
+  <si>
+    <t>Cart</t>
+  </si>
+  <si>
+    <t>Wagon</t>
+  </si>
+  <si>
+    <t>Crossbow</t>
+  </si>
+  <si>
+    <t>Woodworking</t>
+  </si>
+  <si>
+    <t>Biomes</t>
+  </si>
+  <si>
+    <t>Steppe</t>
+  </si>
+  <si>
+    <t>Mountain</t>
+  </si>
+  <si>
+    <t>Forest</t>
+  </si>
+  <si>
+    <t>Highland</t>
+  </si>
+  <si>
+    <t>Swamp</t>
+  </si>
+  <si>
+    <t>Animals</t>
+  </si>
+  <si>
+    <t>Fiber</t>
+  </si>
+  <si>
+    <t>Ore</t>
+  </si>
+  <si>
+    <t>Rock</t>
+  </si>
+  <si>
+    <t>Dagger</t>
+  </si>
+  <si>
+    <t>Sword</t>
+  </si>
+  <si>
+    <t>Primary</t>
+  </si>
+  <si>
+    <t>Secondary</t>
+  </si>
+  <si>
+    <t>Tertiary</t>
+  </si>
+  <si>
+    <t>Extra</t>
+  </si>
+  <si>
+    <t>Stone</t>
+  </si>
+  <si>
+    <t>Fibre</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Craft Categories</t>
+  </si>
+  <si>
+    <t>Gear</t>
+  </si>
+  <si>
+    <t>Tools</t>
+  </si>
+  <si>
+    <t>Potions</t>
+  </si>
+  <si>
+    <t>Food</t>
+  </si>
+  <si>
+    <t>Gear Locations</t>
+  </si>
+  <si>
+    <t>Legs</t>
+  </si>
+  <si>
+    <t>Arms</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>Belt</t>
+  </si>
+  <si>
+    <t>Cloak</t>
+  </si>
+  <si>
+    <t>Main Hand</t>
+  </si>
+  <si>
+    <t>Neck</t>
+  </si>
+  <si>
+    <t>Ring</t>
+  </si>
+  <si>
+    <t>Hammer</t>
+  </si>
+  <si>
+    <t>Axe</t>
+  </si>
+  <si>
+    <t>Spear</t>
+  </si>
+  <si>
+    <t>Javelin</t>
+  </si>
+  <si>
+    <t>Leatherwork</t>
+  </si>
+  <si>
+    <t>Skinning / Tanning</t>
+  </si>
+  <si>
+    <t>Mining / Smelting</t>
+  </si>
+  <si>
+    <t>Treecutting / Planing</t>
+  </si>
+  <si>
+    <t>Cloth Harvesting / Weaving</t>
+  </si>
+  <si>
+    <t>Thin Hide</t>
+  </si>
+  <si>
+    <t>Medium Hide</t>
+  </si>
+  <si>
+    <t>Thick Hide</t>
+  </si>
+  <si>
+    <t>Soft Leather</t>
+  </si>
+  <si>
+    <t>Cured / Boiled Leather</t>
+  </si>
+  <si>
+    <t>Mace</t>
+  </si>
+  <si>
+    <t>Quarrying / Stonecutting</t>
+  </si>
+  <si>
+    <t>Stoneworker</t>
+  </si>
+  <si>
+    <t>Titanium</t>
+  </si>
+  <si>
+    <t>Mithril</t>
+  </si>
+  <si>
+    <t>Tin (Bronze)</t>
+  </si>
+  <si>
+    <t>Iron (Steel)</t>
+  </si>
+  <si>
+    <t>Orichalcum</t>
+  </si>
+  <si>
+    <t>(Silver, Gold, Brass, Nickel, Platinum, Electrum)</t>
+  </si>
+  <si>
+    <t>Adamantium</t>
+  </si>
+  <si>
+    <t>Quality Ranks</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>(Weak?)</t>
+  </si>
+  <si>
+    <t>Uncommon</t>
+  </si>
+  <si>
+    <t>Rare</t>
+  </si>
+  <si>
+    <t>Exceptional</t>
+  </si>
+  <si>
+    <t>Pristine</t>
+  </si>
+  <si>
+    <t>(Runite, Meterorite)</t>
+  </si>
+  <si>
+    <t>Ore Elemental</t>
+  </si>
+  <si>
+    <t>Wood Elemental</t>
+  </si>
+  <si>
+    <t>Stone Elemental</t>
+  </si>
+  <si>
+    <t>Limestone</t>
+  </si>
+  <si>
+    <t>Sandstone</t>
+  </si>
+  <si>
+    <t>Travertine</t>
+  </si>
+  <si>
+    <t>Granite</t>
+  </si>
+  <si>
+    <t>Slate</t>
+  </si>
+  <si>
+    <t>Basalt</t>
+  </si>
+  <si>
+    <t>Marble</t>
+  </si>
+  <si>
+    <t>Chestnut</t>
+  </si>
+  <si>
+    <t>Pine</t>
+  </si>
+  <si>
+    <t>Cedar</t>
+  </si>
+  <si>
+    <t>Bloodoak</t>
+  </si>
+  <si>
+    <t>(Elm, Yew Rods, Maple, Oak)</t>
+  </si>
+  <si>
+    <t>Ashenbard</t>
+  </si>
+  <si>
+    <t>Whitewood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Scraps, Rugged, Robust, Resilient, </t>
+  </si>
+  <si>
+    <t>Flax</t>
+  </si>
+  <si>
+    <t>Skyflower</t>
+  </si>
+  <si>
+    <t>Redleaf</t>
+  </si>
+  <si>
+    <t>Sunflax</t>
+  </si>
+  <si>
+    <t>Ghost Hemp</t>
+  </si>
+  <si>
+    <t>Farm Animals</t>
+  </si>
+  <si>
+    <t>Chicken</t>
+  </si>
+  <si>
+    <t>Goat</t>
+  </si>
+  <si>
+    <t>Sheep</t>
+  </si>
+  <si>
+    <t>Cow</t>
+  </si>
+  <si>
+    <t>Ox</t>
+  </si>
+  <si>
+    <t>Horse</t>
+  </si>
+  <si>
+    <t>Goose</t>
+  </si>
+  <si>
+    <t>Pig</t>
+  </si>
+  <si>
+    <t>Fighters Guild</t>
+  </si>
+  <si>
+    <t>Clerics Guild</t>
+  </si>
+  <si>
+    <t>Mages Guild</t>
+  </si>
+  <si>
+    <t>Rogues Underground</t>
+  </si>
+  <si>
+    <t>Lumbermill</t>
+  </si>
+  <si>
+    <t>Weaver</t>
+  </si>
+  <si>
+    <t>Smelter</t>
+  </si>
+  <si>
+    <t>Tanner</t>
+  </si>
+  <si>
+    <t>Toolmaker</t>
+  </si>
+  <si>
+    <t>Blacksmith</t>
+  </si>
+  <si>
+    <t>Stonemason</t>
+  </si>
+  <si>
+    <t>Ferrier (Repairs)</t>
+  </si>
+  <si>
+    <t>Stables</t>
+  </si>
+  <si>
+    <t>Inn</t>
+  </si>
+  <si>
+    <t>Mill</t>
+  </si>
+  <si>
+    <t>Butcher</t>
+  </si>
+  <si>
+    <t>Baker</t>
+  </si>
+  <si>
+    <t>Herbalist</t>
+  </si>
+  <si>
+    <t>General Store</t>
+  </si>
+  <si>
+    <t>Alchemist</t>
+  </si>
+  <si>
+    <t>Residence</t>
+  </si>
+  <si>
+    <t>Temple</t>
+  </si>
+  <si>
+    <t>Barracks</t>
+  </si>
+  <si>
+    <t>Keep</t>
+  </si>
+  <si>
+    <t>Tailor</t>
+  </si>
+  <si>
+    <t>Leatherworker</t>
+  </si>
+  <si>
+    <t>Grocer</t>
+  </si>
+  <si>
+    <t>Wild Animals</t>
+  </si>
+  <si>
+    <t>Rabbit</t>
+  </si>
+  <si>
+    <t>Deer</t>
+  </si>
+  <si>
+    <t>Fox</t>
+  </si>
+  <si>
+    <t>Wolf</t>
+  </si>
+  <si>
+    <t>Boar</t>
+  </si>
+  <si>
+    <t>Bear</t>
+  </si>
+  <si>
+    <t>Snake</t>
+  </si>
+  <si>
+    <t>Cougar</t>
+  </si>
+  <si>
+    <t>Stag</t>
+  </si>
+  <si>
+    <t>Giant Toad</t>
+  </si>
+  <si>
+    <t>Giant Spider</t>
+  </si>
+  <si>
+    <t>Giant Hornet</t>
+  </si>
+  <si>
+    <t>Giant Lizard</t>
+  </si>
+  <si>
+    <t>Moose</t>
+  </si>
+  <si>
+    <t>Elk</t>
+  </si>
+  <si>
+    <t>Arcane Agaric (Mushroom)</t>
+  </si>
+  <si>
+    <t>Brightleaf Comfrey (Flower)</t>
+  </si>
+  <si>
+    <t>Dragon Teasel (Flower)</t>
+  </si>
+  <si>
+    <t>Crenellated Burdock (Flower)</t>
+  </si>
+  <si>
+    <t>Elusive Foxglove (Flower)</t>
+  </si>
+  <si>
+    <t>Firetouched Mullein (Flower)</t>
+  </si>
+  <si>
+    <t>Ghoul Yarrow (Flower)</t>
+  </si>
+  <si>
+    <t>Healing Potion</t>
+  </si>
+  <si>
+    <t>Energy Potion</t>
+  </si>
+  <si>
+    <t>Stamina Potion</t>
+  </si>
+  <si>
+    <t>Mana Potion</t>
+  </si>
+  <si>
+    <t>Resistance Potion</t>
+  </si>
+  <si>
+    <t>Poison</t>
+  </si>
+  <si>
+    <t>Invisibility</t>
   </si>
 </sst>
 </file>
@@ -1466,37 +2033,49 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1517,35 +2096,23 @@
     <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1881,7 +2448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F86FC45-D7D5-4164-8A37-790C1A972BE9}">
   <dimension ref="A1:AO52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H40" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="Z53" sqref="Z53"/>
     </sheetView>
   </sheetViews>
@@ -1891,135 +2458,135 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="17" t="s">
         <v>318</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
       <c r="T1" s="13"/>
       <c r="U1" s="12"/>
-      <c r="V1" s="39" t="s">
+      <c r="V1" s="17" t="s">
         <v>319</v>
       </c>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-      <c r="Y1" s="39"/>
-      <c r="Z1" s="39"/>
-      <c r="AA1" s="39"/>
-      <c r="AB1" s="39"/>
-      <c r="AC1" s="39"/>
-      <c r="AD1" s="39"/>
-      <c r="AE1" s="39"/>
-      <c r="AF1" s="39"/>
-      <c r="AG1" s="39"/>
-      <c r="AH1" s="39"/>
-      <c r="AI1" s="39"/>
-      <c r="AJ1" s="39"/>
-      <c r="AK1" s="39"/>
-      <c r="AL1" s="39"/>
-      <c r="AM1" s="39"/>
-      <c r="AN1" s="39"/>
-      <c r="AO1" s="39"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="17"/>
+      <c r="AI1" s="17"/>
+      <c r="AJ1" s="17"/>
+      <c r="AK1" s="17"/>
+      <c r="AL1" s="17"/>
+      <c r="AM1" s="17"/>
+      <c r="AN1" s="17"/>
+      <c r="AO1" s="17"/>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="U2" s="12"/>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="37" t="s">
+      <c r="B3" s="21"/>
+      <c r="C3" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37" t="s">
+      <c r="D3" s="18"/>
+      <c r="E3" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37" t="s">
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37" t="s">
+      <c r="I3" s="18"/>
+      <c r="J3" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="K3" s="37"/>
-      <c r="L3" s="37" t="s">
+      <c r="K3" s="18"/>
+      <c r="L3" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="M3" s="37"/>
-      <c r="N3" s="37"/>
-      <c r="O3" s="37" t="s">
+      <c r="M3" s="18"/>
+      <c r="N3" s="18"/>
+      <c r="O3" s="18" t="s">
         <v>277</v>
       </c>
-      <c r="P3" s="37"/>
-      <c r="Q3" s="37" t="s">
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18" t="s">
         <v>280</v>
       </c>
-      <c r="R3" s="37"/>
-      <c r="S3" s="37"/>
+      <c r="R3" s="18"/>
+      <c r="S3" s="18"/>
       <c r="U3" s="12"/>
-      <c r="V3" s="40" t="s">
+      <c r="V3" s="21" t="s">
         <v>271</v>
       </c>
-      <c r="W3" s="40"/>
-      <c r="X3" s="37" t="s">
+      <c r="W3" s="21"/>
+      <c r="X3" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="Y3" s="41"/>
-      <c r="Z3" s="37" t="s">
+      <c r="Y3" s="29"/>
+      <c r="Z3" s="18" t="s">
         <v>320</v>
       </c>
-      <c r="AA3" s="37"/>
-      <c r="AB3" s="37"/>
-      <c r="AC3" s="37"/>
-      <c r="AD3" s="37" t="s">
+      <c r="AA3" s="18"/>
+      <c r="AB3" s="18"/>
+      <c r="AC3" s="18"/>
+      <c r="AD3" s="18" t="s">
         <v>321</v>
       </c>
-      <c r="AE3" s="37"/>
-      <c r="AF3" s="37"/>
-      <c r="AG3" s="37"/>
-      <c r="AH3" s="37" t="s">
+      <c r="AE3" s="18"/>
+      <c r="AF3" s="18"/>
+      <c r="AG3" s="18"/>
+      <c r="AH3" s="18" t="s">
         <v>322</v>
       </c>
-      <c r="AI3" s="37"/>
-      <c r="AJ3" s="37"/>
-      <c r="AK3" s="37"/>
-      <c r="AL3" s="37" t="s">
+      <c r="AI3" s="18"/>
+      <c r="AJ3" s="18"/>
+      <c r="AK3" s="18"/>
+      <c r="AL3" s="18" t="s">
         <v>311</v>
       </c>
-      <c r="AM3" s="37"/>
-      <c r="AN3" s="37"/>
-      <c r="AO3" s="37"/>
+      <c r="AM3" s="18"/>
+      <c r="AN3" s="18"/>
+      <c r="AO3" s="18"/>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="18" t="s">
         <v>278</v>
       </c>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37" t="s">
+      <c r="D4" s="18"/>
+      <c r="E4" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="37"/>
+      <c r="F4" s="18"/>
+      <c r="G4" s="18"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14"/>
@@ -2033,26 +2600,26 @@
       <c r="R4" s="14"/>
       <c r="S4" s="14"/>
       <c r="U4" s="12"/>
-      <c r="X4" s="37" t="s">
+      <c r="X4" s="18" t="s">
         <v>279</v>
       </c>
-      <c r="Y4" s="37"/>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="37" t="s">
+      <c r="Y4" s="18"/>
+      <c r="Z4" s="30"/>
+      <c r="AA4" s="18" t="s">
         <v>323</v>
       </c>
-      <c r="AB4" s="37"/>
-      <c r="AC4" s="38"/>
-      <c r="AD4" s="37" t="s">
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="18" t="s">
         <v>324</v>
       </c>
-      <c r="AE4" s="37"/>
-      <c r="AF4" s="38"/>
-      <c r="AG4" s="37" t="s">
+      <c r="AE4" s="18"/>
+      <c r="AF4" s="30"/>
+      <c r="AG4" s="18" t="s">
         <v>325</v>
       </c>
-      <c r="AH4" s="37"/>
-      <c r="AI4" s="38"/>
+      <c r="AH4" s="18"/>
+      <c r="AI4" s="30"/>
       <c r="AJ4" s="14"/>
       <c r="AK4" s="14"/>
       <c r="AL4" s="14"/>
@@ -2063,820 +2630,820 @@
       <c r="U5" s="12"/>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="19" t="s">
         <v>281</v>
       </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
       <c r="U6" s="12"/>
-      <c r="V6" s="39" t="s">
+      <c r="V6" s="17" t="s">
         <v>326</v>
       </c>
-      <c r="W6" s="39"/>
-      <c r="X6" s="39"/>
-      <c r="Y6" s="39"/>
-      <c r="Z6" s="39"/>
-      <c r="AA6" s="39"/>
-      <c r="AB6" s="39"/>
-      <c r="AC6" s="39"/>
-      <c r="AD6" s="39"/>
-      <c r="AE6" s="39"/>
-      <c r="AF6" s="39"/>
-      <c r="AG6" s="39"/>
-      <c r="AH6" s="39"/>
-      <c r="AI6" s="39"/>
-      <c r="AJ6" s="39"/>
-      <c r="AK6" s="39"/>
-      <c r="AL6" s="39"/>
-      <c r="AM6" s="39"/>
-      <c r="AN6" s="39"/>
-      <c r="AO6" s="39"/>
+      <c r="W6" s="17"/>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17"/>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="17"/>
+      <c r="AC6" s="17"/>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="17"/>
+      <c r="AF6" s="17"/>
+      <c r="AG6" s="17"/>
+      <c r="AH6" s="17"/>
+      <c r="AI6" s="17"/>
+      <c r="AJ6" s="17"/>
+      <c r="AK6" s="17"/>
+      <c r="AL6" s="17"/>
+      <c r="AM6" s="17"/>
+      <c r="AN6" s="17"/>
+      <c r="AO6" s="17"/>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="19" t="s">
         <v>282</v>
       </c>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
       <c r="U7" s="12"/>
-      <c r="V7" s="26" t="s">
+      <c r="V7" s="20" t="s">
         <v>327</v>
       </c>
-      <c r="W7" s="26"/>
-      <c r="X7" s="26"/>
-      <c r="Y7" s="26"/>
-      <c r="Z7" s="20" t="s">
+      <c r="W7" s="20"/>
+      <c r="X7" s="20"/>
+      <c r="Y7" s="20"/>
+      <c r="Z7" s="25" t="s">
         <v>302</v>
       </c>
-      <c r="AA7" s="20"/>
-      <c r="AB7" s="20"/>
-      <c r="AC7" s="34" t="s">
+      <c r="AA7" s="25"/>
+      <c r="AB7" s="25"/>
+      <c r="AC7" s="22" t="s">
         <v>303</v>
       </c>
-      <c r="AD7" s="35"/>
-      <c r="AE7" s="35"/>
-      <c r="AF7" s="35"/>
-      <c r="AG7" s="35"/>
-      <c r="AH7" s="36"/>
+      <c r="AD7" s="23"/>
+      <c r="AE7" s="23"/>
+      <c r="AF7" s="23"/>
+      <c r="AG7" s="23"/>
+      <c r="AH7" s="24"/>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="U8" s="12"/>
-      <c r="AC8" s="34" t="s">
+      <c r="AC8" s="22" t="s">
         <v>328</v>
       </c>
-      <c r="AD8" s="35"/>
-      <c r="AE8" s="35"/>
-      <c r="AF8" s="35"/>
-      <c r="AG8" s="35"/>
-      <c r="AH8" s="36"/>
+      <c r="AD8" s="23"/>
+      <c r="AE8" s="23"/>
+      <c r="AF8" s="23"/>
+      <c r="AG8" s="23"/>
+      <c r="AH8" s="24"/>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="28" t="s">
         <v>283</v>
       </c>
-      <c r="B9" s="24"/>
-      <c r="C9" s="24" t="s">
+      <c r="B9" s="28"/>
+      <c r="C9" s="28" t="s">
         <v>284</v>
       </c>
-      <c r="D9" s="24"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="11">
         <v>10</v>
       </c>
       <c r="U9" s="12"/>
-      <c r="AC9" s="34" t="s">
+      <c r="AC9" s="22" t="s">
         <v>329</v>
       </c>
-      <c r="AD9" s="35"/>
-      <c r="AE9" s="35"/>
-      <c r="AF9" s="35"/>
-      <c r="AG9" s="35"/>
-      <c r="AH9" s="36"/>
+      <c r="AD9" s="23"/>
+      <c r="AE9" s="23"/>
+      <c r="AF9" s="23"/>
+      <c r="AG9" s="23"/>
+      <c r="AH9" s="24"/>
     </row>
     <row r="10" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="28" t="s">
         <v>285</v>
       </c>
-      <c r="B10" s="24"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24" t="s">
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="E10" s="24"/>
-      <c r="F10" s="25" t="s">
+      <c r="E10" s="28"/>
+      <c r="F10" s="27" t="s">
         <v>287</v>
       </c>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="27"/>
+      <c r="L10" s="27"/>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="27"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="27"/>
       <c r="U10" s="12"/>
       <c r="AC10" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="AD10" s="30" t="s">
+      <c r="AD10" s="34" t="s">
         <v>331</v>
       </c>
-      <c r="AE10" s="31"/>
-      <c r="AF10" s="31"/>
-      <c r="AG10" s="32"/>
+      <c r="AE10" s="35"/>
+      <c r="AF10" s="35"/>
+      <c r="AG10" s="36"/>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="F11" s="43" t="s">
+      <c r="F11" s="26" t="s">
         <v>299</v>
       </c>
-      <c r="G11" s="43"/>
-      <c r="H11" s="43" t="s">
+      <c r="G11" s="26"/>
+      <c r="H11" s="26" t="s">
         <v>300</v>
       </c>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="43"/>
-      <c r="L11" s="43" t="s">
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26" t="s">
         <v>298</v>
       </c>
-      <c r="M11" s="43"/>
-      <c r="N11" s="43" t="s">
+      <c r="M11" s="26"/>
+      <c r="N11" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="O11" s="43"/>
-      <c r="P11" s="43"/>
-      <c r="Q11" s="43"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
       <c r="U11" s="12"/>
       <c r="AC11" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="AD11" s="28" t="s">
+      <c r="AD11" s="32" t="s">
         <v>333</v>
       </c>
-      <c r="AE11" s="28"/>
-      <c r="AF11" s="28"/>
-      <c r="AG11" s="28"/>
+      <c r="AE11" s="32"/>
+      <c r="AF11" s="32"/>
+      <c r="AG11" s="32"/>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="U12" s="12"/>
       <c r="AC12" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="AD12" s="28" t="s">
+      <c r="AD12" s="32" t="s">
         <v>335</v>
       </c>
-      <c r="AE12" s="28"/>
-      <c r="AF12" s="28"/>
-      <c r="AG12" s="28"/>
+      <c r="AE12" s="32"/>
+      <c r="AF12" s="32"/>
+      <c r="AG12" s="32"/>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
+      <c r="A13" s="28" t="s">
         <v>288</v>
       </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="25" t="s">
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="27" t="s">
         <v>289</v>
       </c>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
+      <c r="E13" s="27"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="27"/>
+      <c r="H13" s="27"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="27"/>
       <c r="U13" s="12"/>
       <c r="AC13" s="15" t="s">
         <v>336</v>
       </c>
-      <c r="AD13" s="28" t="s">
+      <c r="AD13" s="32" t="s">
         <v>337</v>
       </c>
-      <c r="AE13" s="28"/>
-      <c r="AF13" s="28"/>
-      <c r="AG13" s="28"/>
+      <c r="AE13" s="32"/>
+      <c r="AF13" s="32"/>
+      <c r="AG13" s="32"/>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A14" s="24" t="s">
+      <c r="A14" s="28" t="s">
         <v>290</v>
       </c>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24" t="s">
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="28" t="s">
         <v>286</v>
       </c>
-      <c r="E14" s="24"/>
-      <c r="F14" s="25" t="s">
+      <c r="E14" s="28"/>
+      <c r="F14" s="27" t="s">
         <v>291</v>
       </c>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
+      <c r="G14" s="27"/>
+      <c r="H14" s="27"/>
+      <c r="I14" s="27"/>
+      <c r="J14" s="27"/>
       <c r="U14" s="12"/>
       <c r="AC14" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="AD14" s="29" t="s">
+      <c r="AD14" s="33" t="s">
         <v>339</v>
       </c>
-      <c r="AE14" s="29"/>
-      <c r="AF14" s="29"/>
-      <c r="AG14" s="29"/>
+      <c r="AE14" s="33"/>
+      <c r="AF14" s="33"/>
+      <c r="AG14" s="33"/>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A15" s="24" t="s">
+      <c r="A15" s="28" t="s">
         <v>292</v>
       </c>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25" t="s">
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="27" t="s">
         <v>293</v>
       </c>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
+      <c r="J15" s="27"/>
       <c r="U15" s="12"/>
-      <c r="AC15" s="24" t="s">
+      <c r="AC15" s="28" t="s">
         <v>340</v>
       </c>
-      <c r="AD15" s="24"/>
-      <c r="AE15" s="25" t="s">
+      <c r="AD15" s="28"/>
+      <c r="AE15" s="27" t="s">
         <v>341</v>
       </c>
-      <c r="AF15" s="25"/>
-      <c r="AG15" s="25"/>
-      <c r="AH15" s="25"/>
-      <c r="AI15" s="25"/>
-      <c r="AJ15" s="25"/>
+      <c r="AF15" s="27"/>
+      <c r="AG15" s="27"/>
+      <c r="AH15" s="27"/>
+      <c r="AI15" s="27"/>
+      <c r="AJ15" s="27"/>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="19"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="19"/>
       <c r="U16" s="12"/>
-      <c r="V16" s="33" t="s">
+      <c r="V16" s="37" t="s">
         <v>349</v>
       </c>
-      <c r="W16" s="33"/>
-      <c r="X16" s="33"/>
-      <c r="Y16" s="33"/>
-      <c r="Z16" s="33"/>
-      <c r="AA16" s="33"/>
-      <c r="AC16" s="23" t="s">
+      <c r="W16" s="37"/>
+      <c r="X16" s="37"/>
+      <c r="Y16" s="37"/>
+      <c r="Z16" s="37"/>
+      <c r="AA16" s="37"/>
+      <c r="AC16" s="39" t="s">
         <v>342</v>
       </c>
-      <c r="AD16" s="23"/>
-      <c r="AE16" s="23"/>
-      <c r="AF16" s="20" t="s">
+      <c r="AD16" s="39"/>
+      <c r="AE16" s="39"/>
+      <c r="AF16" s="25" t="s">
         <v>343</v>
       </c>
-      <c r="AG16" s="20"/>
-      <c r="AH16" s="20"/>
-      <c r="AI16" s="20"/>
-      <c r="AJ16" s="20"/>
+      <c r="AG16" s="25"/>
+      <c r="AH16" s="25"/>
+      <c r="AI16" s="25"/>
+      <c r="AJ16" s="25"/>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
       <c r="U17" s="12"/>
-      <c r="V17" s="33" t="s">
+      <c r="V17" s="37" t="s">
         <v>350</v>
       </c>
-      <c r="W17" s="33"/>
-      <c r="X17" s="33"/>
-      <c r="Y17" s="33"/>
-      <c r="Z17" s="33"/>
-      <c r="AA17" s="33"/>
-      <c r="AC17" s="23" t="s">
+      <c r="W17" s="37"/>
+      <c r="X17" s="37"/>
+      <c r="Y17" s="37"/>
+      <c r="Z17" s="37"/>
+      <c r="AA17" s="37"/>
+      <c r="AC17" s="39" t="s">
         <v>344</v>
       </c>
-      <c r="AD17" s="23"/>
-      <c r="AE17" s="23"/>
-      <c r="AF17" s="20" t="s">
+      <c r="AD17" s="39"/>
+      <c r="AE17" s="39"/>
+      <c r="AF17" s="25" t="s">
         <v>345</v>
       </c>
-      <c r="AG17" s="20"/>
-      <c r="AH17" s="20"/>
-      <c r="AI17" s="20"/>
-      <c r="AJ17" s="20"/>
+      <c r="AG17" s="25"/>
+      <c r="AH17" s="25"/>
+      <c r="AI17" s="25"/>
+      <c r="AJ17" s="25"/>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A18" s="26" t="s">
+      <c r="A18" s="20" t="s">
         <v>295</v>
       </c>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="17" t="s">
+      <c r="B18" s="20"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="19" t="s">
         <v>296</v>
       </c>
-      <c r="F18" s="17"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
       <c r="U18" s="12"/>
-      <c r="V18" s="33" t="s">
+      <c r="V18" s="37" t="s">
         <v>351</v>
       </c>
-      <c r="W18" s="33"/>
-      <c r="X18" s="33"/>
-      <c r="Y18" s="33"/>
-      <c r="Z18" s="33"/>
-      <c r="AA18" s="33"/>
-      <c r="AC18" s="23" t="s">
+      <c r="W18" s="37"/>
+      <c r="X18" s="37"/>
+      <c r="Y18" s="37"/>
+      <c r="Z18" s="37"/>
+      <c r="AA18" s="37"/>
+      <c r="AC18" s="39" t="s">
         <v>354</v>
       </c>
-      <c r="AD18" s="23"/>
-      <c r="AE18" s="23"/>
-      <c r="AF18" s="20" t="s">
+      <c r="AD18" s="39"/>
+      <c r="AE18" s="39"/>
+      <c r="AF18" s="25" t="s">
         <v>346</v>
       </c>
-      <c r="AG18" s="20"/>
-      <c r="AH18" s="20"/>
-      <c r="AI18" s="20"/>
-      <c r="AJ18" s="20"/>
+      <c r="AG18" s="25"/>
+      <c r="AH18" s="25"/>
+      <c r="AI18" s="25"/>
+      <c r="AJ18" s="25"/>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="E19" s="17" t="s">
+      <c r="E19" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
-      <c r="K19" s="42"/>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
+      <c r="J19" s="31"/>
+      <c r="K19" s="31"/>
       <c r="U19" s="12"/>
-      <c r="V19" s="33" t="s">
+      <c r="V19" s="37" t="s">
         <v>352</v>
       </c>
-      <c r="W19" s="33"/>
-      <c r="X19" s="33"/>
-      <c r="Y19" s="33"/>
-      <c r="Z19" s="33"/>
-      <c r="AA19" s="33"/>
-      <c r="AC19" s="23" t="s">
+      <c r="W19" s="37"/>
+      <c r="X19" s="37"/>
+      <c r="Y19" s="37"/>
+      <c r="Z19" s="37"/>
+      <c r="AA19" s="37"/>
+      <c r="AC19" s="39" t="s">
         <v>347</v>
       </c>
-      <c r="AD19" s="23"/>
-      <c r="AE19" s="23"/>
-      <c r="AF19" s="20" t="s">
+      <c r="AD19" s="39"/>
+      <c r="AE19" s="39"/>
+      <c r="AF19" s="25" t="s">
         <v>346</v>
       </c>
-      <c r="AG19" s="20"/>
-      <c r="AH19" s="20"/>
-      <c r="AI19" s="20"/>
-      <c r="AJ19" s="20"/>
+      <c r="AG19" s="25"/>
+      <c r="AH19" s="25"/>
+      <c r="AI19" s="25"/>
+      <c r="AJ19" s="25"/>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="25" t="s">
         <v>302</v>
       </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="34" t="s">
+      <c r="F20" s="25"/>
+      <c r="G20" s="25"/>
+      <c r="H20" s="22" t="s">
         <v>303</v>
       </c>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="36"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="24"/>
       <c r="U20" s="12"/>
-      <c r="V20" s="33" t="s">
+      <c r="V20" s="37" t="s">
         <v>353</v>
       </c>
-      <c r="W20" s="33"/>
-      <c r="X20" s="33"/>
-      <c r="Y20" s="33"/>
-      <c r="Z20" s="33"/>
-      <c r="AA20" s="33"/>
-      <c r="AC20" s="23" t="s">
+      <c r="W20" s="37"/>
+      <c r="X20" s="37"/>
+      <c r="Y20" s="37"/>
+      <c r="Z20" s="37"/>
+      <c r="AA20" s="37"/>
+      <c r="AC20" s="39" t="s">
         <v>348</v>
       </c>
-      <c r="AD20" s="23"/>
-      <c r="AE20" s="23"/>
-      <c r="AF20" s="20" t="s">
+      <c r="AD20" s="39"/>
+      <c r="AE20" s="39"/>
+      <c r="AF20" s="25" t="s">
         <v>308</v>
       </c>
-      <c r="AG20" s="20"/>
-      <c r="AH20" s="20"/>
-      <c r="AI20" s="20"/>
-      <c r="AJ20" s="20"/>
+      <c r="AG20" s="25"/>
+      <c r="AH20" s="25"/>
+      <c r="AI20" s="25"/>
+      <c r="AJ20" s="25"/>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="H21" s="34" t="s">
+      <c r="H21" s="22" t="s">
         <v>304</v>
       </c>
-      <c r="I21" s="35"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="35"/>
-      <c r="M21" s="36"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="24"/>
       <c r="U21" s="12"/>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="H22" s="34" t="s">
+      <c r="H22" s="22" t="s">
         <v>313</v>
       </c>
-      <c r="I22" s="35"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="35"/>
-      <c r="L22" s="35"/>
-      <c r="M22" s="36"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="24"/>
       <c r="U22" s="12"/>
-      <c r="V22" s="26" t="s">
+      <c r="V22" s="20" t="s">
         <v>355</v>
       </c>
-      <c r="W22" s="26"/>
-      <c r="X22" s="26"/>
-      <c r="Y22" s="26"/>
-      <c r="Z22" s="17" t="s">
+      <c r="W22" s="20"/>
+      <c r="X22" s="20"/>
+      <c r="Y22" s="20"/>
+      <c r="Z22" s="19" t="s">
         <v>359</v>
       </c>
-      <c r="AA22" s="17"/>
-      <c r="AB22" s="17"/>
-      <c r="AC22" s="17"/>
-      <c r="AD22" s="17"/>
-      <c r="AE22" s="17"/>
-      <c r="AF22" s="17"/>
-      <c r="AG22" s="17"/>
-      <c r="AH22" s="17"/>
-      <c r="AI22" s="17"/>
-      <c r="AJ22" s="17"/>
+      <c r="AA22" s="19"/>
+      <c r="AB22" s="19"/>
+      <c r="AC22" s="19"/>
+      <c r="AD22" s="19"/>
+      <c r="AE22" s="19"/>
+      <c r="AF22" s="19"/>
+      <c r="AG22" s="19"/>
+      <c r="AH22" s="19"/>
+      <c r="AI22" s="19"/>
+      <c r="AJ22" s="19"/>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="K23" s="17" t="s">
+      <c r="K23" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="L23" s="17"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
-      <c r="P23" s="17"/>
-      <c r="Q23" s="17"/>
-      <c r="R23" s="17"/>
+      <c r="L23" s="19"/>
+      <c r="M23" s="19"/>
+      <c r="N23" s="19"/>
+      <c r="O23" s="19"/>
+      <c r="P23" s="19"/>
+      <c r="Q23" s="19"/>
+      <c r="R23" s="19"/>
       <c r="U23" s="12"/>
-      <c r="Z23" s="20" t="s">
+      <c r="Z23" s="25" t="s">
         <v>302</v>
       </c>
-      <c r="AA23" s="20"/>
-      <c r="AB23" s="20"/>
-      <c r="AC23" s="27" t="s">
+      <c r="AA23" s="25"/>
+      <c r="AB23" s="25"/>
+      <c r="AC23" s="38" t="s">
         <v>360</v>
       </c>
-      <c r="AD23" s="27"/>
-      <c r="AE23" s="25" t="s">
+      <c r="AD23" s="38"/>
+      <c r="AE23" s="27" t="s">
         <v>361</v>
       </c>
-      <c r="AF23" s="25"/>
-      <c r="AG23" s="25"/>
-      <c r="AH23" s="25"/>
-      <c r="AI23" s="25"/>
-      <c r="AJ23" s="25"/>
+      <c r="AF23" s="27"/>
+      <c r="AG23" s="27"/>
+      <c r="AH23" s="27"/>
+      <c r="AI23" s="27"/>
+      <c r="AJ23" s="27"/>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="K24" s="42" t="s">
+      <c r="K24" s="31" t="s">
         <v>312</v>
       </c>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
-      <c r="N24" s="17"/>
-      <c r="O24" s="17"/>
-      <c r="P24" s="17"/>
-      <c r="Q24" s="17"/>
-      <c r="R24" s="17"/>
+      <c r="L24" s="31"/>
+      <c r="M24" s="31"/>
+      <c r="N24" s="19"/>
+      <c r="O24" s="19"/>
+      <c r="P24" s="19"/>
+      <c r="Q24" s="19"/>
+      <c r="R24" s="19"/>
       <c r="U24" s="12"/>
-      <c r="AC24" s="21" t="s">
+      <c r="AC24" s="42" t="s">
         <v>362</v>
       </c>
-      <c r="AD24" s="21"/>
-      <c r="AE24" s="21"/>
-      <c r="AF24" s="21"/>
-      <c r="AG24" s="22" t="s">
+      <c r="AD24" s="42"/>
+      <c r="AE24" s="42"/>
+      <c r="AF24" s="42"/>
+      <c r="AG24" s="41" t="s">
         <v>363</v>
       </c>
-      <c r="AH24" s="22"/>
-      <c r="AI24" s="22"/>
+      <c r="AH24" s="41"/>
+      <c r="AI24" s="41"/>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="H25" s="17" t="s">
+      <c r="H25" s="19" t="s">
         <v>314</v>
       </c>
-      <c r="I25" s="17"/>
-      <c r="J25" s="17"/>
-      <c r="K25" s="42"/>
-      <c r="L25" s="42"/>
-      <c r="M25" s="42"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="31"/>
+      <c r="L25" s="31"/>
+      <c r="M25" s="31"/>
       <c r="U25" s="12"/>
-      <c r="AC25" s="23" t="s">
+      <c r="AC25" s="39" t="s">
         <v>369</v>
       </c>
-      <c r="AD25" s="23"/>
-      <c r="AE25" s="23"/>
-      <c r="AF25" s="23"/>
-      <c r="AG25" s="23"/>
-      <c r="AH25" s="23"/>
-      <c r="AI25" s="23"/>
-      <c r="AJ25" s="23"/>
+      <c r="AD25" s="39"/>
+      <c r="AE25" s="39"/>
+      <c r="AF25" s="39"/>
+      <c r="AG25" s="39"/>
+      <c r="AH25" s="39"/>
+      <c r="AI25" s="39"/>
+      <c r="AJ25" s="39"/>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="K26" s="17" t="s">
+      <c r="K26" s="19" t="s">
         <v>315</v>
       </c>
-      <c r="L26" s="17"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
-      <c r="P26" s="17"/>
-      <c r="Q26" s="17"/>
-      <c r="R26" s="17"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+      <c r="N26" s="19"/>
+      <c r="O26" s="19"/>
+      <c r="P26" s="19"/>
+      <c r="Q26" s="19"/>
+      <c r="R26" s="19"/>
       <c r="U26" s="12"/>
-      <c r="AG26" s="17" t="s">
+      <c r="AG26" s="19" t="s">
         <v>364</v>
       </c>
-      <c r="AH26" s="17"/>
-      <c r="AI26" s="17"/>
-      <c r="AJ26" s="17"/>
+      <c r="AH26" s="19"/>
+      <c r="AI26" s="19"/>
+      <c r="AJ26" s="19"/>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="K27" s="17" t="s">
+      <c r="K27" s="19" t="s">
         <v>316</v>
       </c>
-      <c r="L27" s="17"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
-      <c r="P27" s="17"/>
-      <c r="Q27" s="17"/>
-      <c r="R27" s="17"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+      <c r="N27" s="19"/>
+      <c r="O27" s="19"/>
+      <c r="P27" s="19"/>
+      <c r="Q27" s="19"/>
+      <c r="R27" s="19"/>
       <c r="U27" s="12"/>
-      <c r="AC27" s="24" t="s">
+      <c r="AC27" s="28" t="s">
         <v>360</v>
       </c>
-      <c r="AD27" s="24"/>
-      <c r="AE27" s="25" t="s">
+      <c r="AD27" s="28"/>
+      <c r="AE27" s="27" t="s">
         <v>365</v>
       </c>
-      <c r="AF27" s="25"/>
-      <c r="AG27" s="25"/>
-      <c r="AH27" s="25"/>
-      <c r="AI27" s="25"/>
-      <c r="AJ27" s="25"/>
-      <c r="AK27" s="25"/>
-      <c r="AL27" s="25"/>
+      <c r="AF27" s="27"/>
+      <c r="AG27" s="27"/>
+      <c r="AH27" s="27"/>
+      <c r="AI27" s="27"/>
+      <c r="AJ27" s="27"/>
+      <c r="AK27" s="27"/>
+      <c r="AL27" s="27"/>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="K28" s="17" t="s">
+      <c r="K28" s="19" t="s">
         <v>317</v>
       </c>
-      <c r="L28" s="17"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="17"/>
-      <c r="O28" s="17"/>
-      <c r="P28" s="17"/>
-      <c r="Q28" s="17"/>
-      <c r="R28" s="17"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+      <c r="N28" s="19"/>
+      <c r="O28" s="19"/>
+      <c r="P28" s="19"/>
+      <c r="Q28" s="19"/>
+      <c r="R28" s="19"/>
       <c r="U28" s="12"/>
-      <c r="AC28" s="17" t="s">
+      <c r="AC28" s="19" t="s">
         <v>328</v>
       </c>
-      <c r="AD28" s="17"/>
-      <c r="AE28" s="18"/>
-      <c r="AF28" s="18"/>
-      <c r="AG28" s="18"/>
+      <c r="AD28" s="19"/>
+      <c r="AE28" s="43"/>
+      <c r="AF28" s="43"/>
+      <c r="AG28" s="43"/>
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="H29" s="20" t="s">
+      <c r="H29" s="25" t="s">
         <v>305</v>
       </c>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="17" t="s">
+      <c r="I29" s="25"/>
+      <c r="J29" s="25"/>
+      <c r="K29" s="25"/>
+      <c r="L29" s="25"/>
+      <c r="M29" s="19" t="s">
         <v>306</v>
       </c>
-      <c r="N29" s="17"/>
-      <c r="O29" s="17"/>
-      <c r="P29" s="17"/>
-      <c r="Q29" s="17"/>
-      <c r="R29" s="17"/>
+      <c r="N29" s="19"/>
+      <c r="O29" s="19"/>
+      <c r="P29" s="19"/>
+      <c r="Q29" s="19"/>
+      <c r="R29" s="19"/>
       <c r="U29" s="12"/>
-      <c r="AC29" s="19" t="s">
+      <c r="AC29" s="40" t="s">
         <v>366</v>
       </c>
-      <c r="AD29" s="19"/>
-      <c r="AE29" s="19"/>
+      <c r="AD29" s="40"/>
+      <c r="AE29" s="40"/>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="M30" s="17" t="s">
+      <c r="M30" s="19" t="s">
         <v>307</v>
       </c>
-      <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
-      <c r="P30" s="17"/>
-      <c r="Q30" s="17"/>
-      <c r="R30" s="17"/>
+      <c r="N30" s="19"/>
+      <c r="O30" s="19"/>
+      <c r="P30" s="19"/>
+      <c r="Q30" s="19"/>
+      <c r="R30" s="19"/>
       <c r="U30" s="12"/>
-      <c r="Z30" s="17" t="s">
+      <c r="Z30" s="19" t="s">
         <v>367</v>
       </c>
-      <c r="AA30" s="17"/>
-      <c r="AB30" s="17"/>
-      <c r="AC30" s="17"/>
-      <c r="AD30" s="17"/>
+      <c r="AA30" s="19"/>
+      <c r="AB30" s="19"/>
+      <c r="AC30" s="19"/>
+      <c r="AD30" s="19"/>
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="M31" s="17" t="s">
+      <c r="M31" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
-      <c r="P31" s="17"/>
-      <c r="Q31" s="17"/>
-      <c r="R31" s="17"/>
+      <c r="N31" s="19"/>
+      <c r="O31" s="19"/>
+      <c r="P31" s="19"/>
+      <c r="Q31" s="19"/>
+      <c r="R31" s="19"/>
       <c r="U31" s="12"/>
-      <c r="Z31" s="19" t="s">
+      <c r="Z31" s="40" t="s">
         <v>368</v>
       </c>
-      <c r="AA31" s="19"/>
-      <c r="AB31" s="19"/>
+      <c r="AA31" s="40"/>
+      <c r="AB31" s="40"/>
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="U32" s="12"/>
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="19" t="s">
         <v>309</v>
       </c>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="17"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
       <c r="U33" s="12"/>
-      <c r="V33" s="26" t="s">
+      <c r="V33" s="20" t="s">
         <v>356</v>
       </c>
-      <c r="W33" s="26"/>
-      <c r="X33" s="26"/>
-      <c r="Y33" s="26"/>
-      <c r="Z33" s="17" t="s">
+      <c r="W33" s="20"/>
+      <c r="X33" s="20"/>
+      <c r="Y33" s="20"/>
+      <c r="Z33" s="19" t="s">
         <v>359</v>
       </c>
-      <c r="AA33" s="17"/>
-      <c r="AB33" s="17"/>
-      <c r="AC33" s="17"/>
-      <c r="AD33" s="17"/>
-      <c r="AE33" s="17"/>
-      <c r="AF33" s="17"/>
-      <c r="AG33" s="17"/>
-      <c r="AH33" s="17"/>
-      <c r="AI33" s="17"/>
-      <c r="AJ33" s="17"/>
+      <c r="AA33" s="19"/>
+      <c r="AB33" s="19"/>
+      <c r="AC33" s="19"/>
+      <c r="AD33" s="19"/>
+      <c r="AE33" s="19"/>
+      <c r="AF33" s="19"/>
+      <c r="AG33" s="19"/>
+      <c r="AH33" s="19"/>
+      <c r="AI33" s="19"/>
+      <c r="AJ33" s="19"/>
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.25">
       <c r="U34" s="12"/>
-      <c r="Z34" s="20" t="s">
+      <c r="Z34" s="25" t="s">
         <v>302</v>
       </c>
-      <c r="AA34" s="20"/>
-      <c r="AB34" s="20"/>
-      <c r="AC34" s="27" t="s">
+      <c r="AA34" s="25"/>
+      <c r="AB34" s="25"/>
+      <c r="AC34" s="38" t="s">
         <v>360</v>
       </c>
-      <c r="AD34" s="27"/>
-      <c r="AE34" s="25" t="s">
+      <c r="AD34" s="38"/>
+      <c r="AE34" s="27" t="s">
         <v>361</v>
       </c>
-      <c r="AF34" s="25"/>
-      <c r="AG34" s="25"/>
-      <c r="AH34" s="25"/>
-      <c r="AI34" s="25"/>
-      <c r="AJ34" s="25"/>
+      <c r="AF34" s="27"/>
+      <c r="AG34" s="27"/>
+      <c r="AH34" s="27"/>
+      <c r="AI34" s="27"/>
+      <c r="AJ34" s="27"/>
     </row>
     <row r="35" spans="1:38" x14ac:dyDescent="0.25">
       <c r="U35" s="12"/>
-      <c r="AC35" s="21" t="s">
+      <c r="AC35" s="42" t="s">
         <v>362</v>
       </c>
-      <c r="AD35" s="21"/>
-      <c r="AE35" s="21"/>
-      <c r="AF35" s="21"/>
-      <c r="AG35" s="22" t="s">
+      <c r="AD35" s="42"/>
+      <c r="AE35" s="42"/>
+      <c r="AF35" s="42"/>
+      <c r="AG35" s="41" t="s">
         <v>363</v>
       </c>
-      <c r="AH35" s="22"/>
-      <c r="AI35" s="22"/>
+      <c r="AH35" s="41"/>
+      <c r="AI35" s="41"/>
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.25">
       <c r="U36" s="12"/>
-      <c r="AC36" s="23" t="s">
+      <c r="AC36" s="39" t="s">
         <v>369</v>
       </c>
-      <c r="AD36" s="23"/>
-      <c r="AE36" s="23"/>
-      <c r="AF36" s="23"/>
-      <c r="AG36" s="23"/>
-      <c r="AH36" s="23"/>
-      <c r="AI36" s="23"/>
-      <c r="AJ36" s="23"/>
+      <c r="AD36" s="39"/>
+      <c r="AE36" s="39"/>
+      <c r="AF36" s="39"/>
+      <c r="AG36" s="39"/>
+      <c r="AH36" s="39"/>
+      <c r="AI36" s="39"/>
+      <c r="AJ36" s="39"/>
     </row>
     <row r="37" spans="1:38" x14ac:dyDescent="0.25">
       <c r="U37" s="12"/>
-      <c r="AG37" s="17" t="s">
+      <c r="AG37" s="19" t="s">
         <v>364</v>
       </c>
-      <c r="AH37" s="17"/>
-      <c r="AI37" s="17"/>
-      <c r="AJ37" s="17"/>
+      <c r="AH37" s="19"/>
+      <c r="AI37" s="19"/>
+      <c r="AJ37" s="19"/>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.25">
       <c r="U38" s="12"/>
-      <c r="AC38" s="24" t="s">
+      <c r="AC38" s="28" t="s">
         <v>360</v>
       </c>
-      <c r="AD38" s="24"/>
-      <c r="AE38" s="25" t="s">
+      <c r="AD38" s="28"/>
+      <c r="AE38" s="27" t="s">
         <v>365</v>
       </c>
-      <c r="AF38" s="25"/>
-      <c r="AG38" s="25"/>
-      <c r="AH38" s="25"/>
-      <c r="AI38" s="25"/>
-      <c r="AJ38" s="25"/>
-      <c r="AK38" s="25"/>
-      <c r="AL38" s="25"/>
+      <c r="AF38" s="27"/>
+      <c r="AG38" s="27"/>
+      <c r="AH38" s="27"/>
+      <c r="AI38" s="27"/>
+      <c r="AJ38" s="27"/>
+      <c r="AK38" s="27"/>
+      <c r="AL38" s="27"/>
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.25">
       <c r="U39" s="12"/>
-      <c r="AC39" s="17" t="s">
+      <c r="AC39" s="19" t="s">
         <v>370</v>
       </c>
-      <c r="AD39" s="17"/>
-      <c r="AE39" s="17"/>
-      <c r="AF39" s="17"/>
-      <c r="AG39" s="17"/>
-      <c r="AH39" s="17" t="s">
+      <c r="AD39" s="19"/>
+      <c r="AE39" s="19"/>
+      <c r="AF39" s="19"/>
+      <c r="AG39" s="19"/>
+      <c r="AH39" s="19" t="s">
         <v>328</v>
       </c>
-      <c r="AI39" s="17"/>
-      <c r="AJ39" s="18"/>
-      <c r="AK39" s="18"/>
-      <c r="AL39" s="18"/>
+      <c r="AI39" s="19"/>
+      <c r="AJ39" s="43"/>
+      <c r="AK39" s="43"/>
+      <c r="AL39" s="43"/>
     </row>
     <row r="40" spans="1:38" x14ac:dyDescent="0.25">
       <c r="U40" s="12"/>
-      <c r="AH40" s="19" t="s">
+      <c r="AH40" s="40" t="s">
         <v>366</v>
       </c>
-      <c r="AI40" s="19"/>
-      <c r="AJ40" s="19"/>
+      <c r="AI40" s="40"/>
+      <c r="AJ40" s="40"/>
     </row>
     <row r="41" spans="1:38" x14ac:dyDescent="0.25">
       <c r="U41" s="12"/>
-      <c r="AC41" s="20" t="s">
+      <c r="AC41" s="25" t="s">
         <v>371</v>
       </c>
-      <c r="AD41" s="20"/>
-      <c r="AE41" s="20" t="s">
+      <c r="AD41" s="25"/>
+      <c r="AE41" s="25" t="s">
         <v>363</v>
       </c>
-      <c r="AF41" s="20"/>
-      <c r="AG41" s="20"/>
+      <c r="AF41" s="25"/>
+      <c r="AG41" s="25"/>
     </row>
     <row r="42" spans="1:38" x14ac:dyDescent="0.25">
       <c r="U42" s="12"/>
-      <c r="Z42" s="20" t="s">
+      <c r="Z42" s="25" t="s">
         <v>368</v>
       </c>
-      <c r="AA42" s="20"/>
-      <c r="AB42" s="20"/>
+      <c r="AA42" s="25"/>
+      <c r="AB42" s="25"/>
     </row>
     <row r="43" spans="1:38" x14ac:dyDescent="0.25">
       <c r="U43" s="12"/>
@@ -2886,16 +3453,16 @@
     </row>
     <row r="45" spans="1:38" x14ac:dyDescent="0.25">
       <c r="U45" s="12"/>
-      <c r="V45" s="26" t="s">
+      <c r="V45" s="20" t="s">
         <v>357</v>
       </c>
-      <c r="W45" s="26"/>
-      <c r="X45" s="26"/>
-      <c r="Y45" s="26"/>
-      <c r="Z45" s="20" t="s">
+      <c r="W45" s="20"/>
+      <c r="X45" s="20"/>
+      <c r="Y45" s="20"/>
+      <c r="Z45" s="25" t="s">
         <v>346</v>
       </c>
-      <c r="AA45" s="20"/>
+      <c r="AA45" s="25"/>
     </row>
     <row r="46" spans="1:38" x14ac:dyDescent="0.25">
       <c r="U46" s="12"/>
@@ -2905,44 +3472,44 @@
     </row>
     <row r="48" spans="1:38" x14ac:dyDescent="0.25">
       <c r="U48" s="12"/>
-      <c r="V48" s="26" t="s">
+      <c r="V48" s="20" t="s">
         <v>358</v>
       </c>
-      <c r="W48" s="26"/>
-      <c r="X48" s="26"/>
-      <c r="Y48" s="26"/>
-      <c r="Z48" s="20" t="s">
+      <c r="W48" s="20"/>
+      <c r="X48" s="20"/>
+      <c r="Y48" s="20"/>
+      <c r="Z48" s="25" t="s">
         <v>346</v>
       </c>
-      <c r="AA48" s="20"/>
+      <c r="AA48" s="25"/>
     </row>
     <row r="49" spans="21:41" x14ac:dyDescent="0.25">
       <c r="U49" s="12"/>
     </row>
     <row r="50" spans="21:41" x14ac:dyDescent="0.25">
       <c r="U50" s="12"/>
-      <c r="V50" s="39" t="s">
+      <c r="V50" s="17" t="s">
         <v>372</v>
       </c>
-      <c r="W50" s="39"/>
-      <c r="X50" s="39"/>
-      <c r="Y50" s="39"/>
-      <c r="Z50" s="39"/>
-      <c r="AA50" s="39"/>
-      <c r="AB50" s="39"/>
-      <c r="AC50" s="39"/>
-      <c r="AD50" s="39"/>
-      <c r="AE50" s="39"/>
-      <c r="AF50" s="39"/>
-      <c r="AG50" s="39"/>
-      <c r="AH50" s="39"/>
-      <c r="AI50" s="39"/>
-      <c r="AJ50" s="39"/>
-      <c r="AK50" s="39"/>
-      <c r="AL50" s="39"/>
-      <c r="AM50" s="39"/>
-      <c r="AN50" s="39"/>
-      <c r="AO50" s="39"/>
+      <c r="W50" s="17"/>
+      <c r="X50" s="17"/>
+      <c r="Y50" s="17"/>
+      <c r="Z50" s="17"/>
+      <c r="AA50" s="17"/>
+      <c r="AB50" s="17"/>
+      <c r="AC50" s="17"/>
+      <c r="AD50" s="17"/>
+      <c r="AE50" s="17"/>
+      <c r="AF50" s="17"/>
+      <c r="AG50" s="17"/>
+      <c r="AH50" s="17"/>
+      <c r="AI50" s="17"/>
+      <c r="AJ50" s="17"/>
+      <c r="AK50" s="17"/>
+      <c r="AL50" s="17"/>
+      <c r="AM50" s="17"/>
+      <c r="AN50" s="17"/>
+      <c r="AO50" s="17"/>
     </row>
     <row r="51" spans="21:41" x14ac:dyDescent="0.25">
       <c r="V51" s="10" t="s">
@@ -2962,6 +3529,106 @@
     </row>
   </sheetData>
   <mergeCells count="124">
+    <mergeCell ref="AH39:AL39"/>
+    <mergeCell ref="AH40:AJ40"/>
+    <mergeCell ref="Z42:AB42"/>
+    <mergeCell ref="AE41:AG41"/>
+    <mergeCell ref="AC41:AD41"/>
+    <mergeCell ref="AC39:AG39"/>
+    <mergeCell ref="AC35:AF35"/>
+    <mergeCell ref="AG35:AI35"/>
+    <mergeCell ref="AC36:AJ36"/>
+    <mergeCell ref="AG37:AJ37"/>
+    <mergeCell ref="AC38:AD38"/>
+    <mergeCell ref="AE38:AL38"/>
+    <mergeCell ref="AE15:AJ15"/>
+    <mergeCell ref="AF16:AJ16"/>
+    <mergeCell ref="AF17:AJ17"/>
+    <mergeCell ref="AF18:AJ18"/>
+    <mergeCell ref="V20:AA20"/>
+    <mergeCell ref="V45:Y45"/>
+    <mergeCell ref="V48:Y48"/>
+    <mergeCell ref="Z45:AA45"/>
+    <mergeCell ref="Z48:AA48"/>
+    <mergeCell ref="Z31:AB31"/>
+    <mergeCell ref="AG24:AI24"/>
+    <mergeCell ref="AE27:AL27"/>
+    <mergeCell ref="AG26:AJ26"/>
+    <mergeCell ref="AC34:AD34"/>
+    <mergeCell ref="AE34:AJ34"/>
+    <mergeCell ref="Z22:AJ22"/>
+    <mergeCell ref="Z33:AJ33"/>
+    <mergeCell ref="Z30:AD30"/>
+    <mergeCell ref="AC29:AE29"/>
+    <mergeCell ref="AC27:AD27"/>
+    <mergeCell ref="AC24:AF24"/>
+    <mergeCell ref="AE23:AJ23"/>
+    <mergeCell ref="AC25:AJ25"/>
+    <mergeCell ref="AC28:AG28"/>
+    <mergeCell ref="V16:AA16"/>
+    <mergeCell ref="V17:AA17"/>
+    <mergeCell ref="V18:AA18"/>
+    <mergeCell ref="V19:AA19"/>
+    <mergeCell ref="AF19:AJ19"/>
+    <mergeCell ref="AF20:AJ20"/>
+    <mergeCell ref="Z23:AB23"/>
+    <mergeCell ref="Z34:AB34"/>
+    <mergeCell ref="V22:Y22"/>
+    <mergeCell ref="V33:Y33"/>
+    <mergeCell ref="AC23:AD23"/>
+    <mergeCell ref="AC16:AE16"/>
+    <mergeCell ref="AC17:AE17"/>
+    <mergeCell ref="AC18:AE18"/>
+    <mergeCell ref="AC19:AE19"/>
+    <mergeCell ref="AC20:AE20"/>
+    <mergeCell ref="M31:R31"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="V3:W3"/>
+    <mergeCell ref="X3:Y3"/>
+    <mergeCell ref="X4:Z4"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="AD3:AG3"/>
+    <mergeCell ref="AH3:AK3"/>
+    <mergeCell ref="K26:R26"/>
+    <mergeCell ref="K27:R27"/>
+    <mergeCell ref="K28:R28"/>
+    <mergeCell ref="H29:L29"/>
+    <mergeCell ref="M30:R30"/>
+    <mergeCell ref="M29:R29"/>
+    <mergeCell ref="K23:R23"/>
+    <mergeCell ref="K24:R24"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="H21:M21"/>
+    <mergeCell ref="H20:M20"/>
+    <mergeCell ref="D15:J15"/>
+    <mergeCell ref="E19:K19"/>
+    <mergeCell ref="E18:K18"/>
+    <mergeCell ref="N11:Q11"/>
+    <mergeCell ref="AC7:AH7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:Q10"/>
+    <mergeCell ref="V1:AO1"/>
+    <mergeCell ref="Z7:AB7"/>
+    <mergeCell ref="V7:Y7"/>
+    <mergeCell ref="AC8:AH8"/>
+    <mergeCell ref="AC9:AH9"/>
+    <mergeCell ref="AL3:AO3"/>
+    <mergeCell ref="AA4:AC4"/>
+    <mergeCell ref="AD4:AF4"/>
+    <mergeCell ref="AG4:AI4"/>
+    <mergeCell ref="V6:AO6"/>
+    <mergeCell ref="AD11:AG11"/>
+    <mergeCell ref="AD12:AG12"/>
+    <mergeCell ref="AD13:AG13"/>
+    <mergeCell ref="AD14:AG14"/>
+    <mergeCell ref="AD10:AG10"/>
+    <mergeCell ref="AC15:AD15"/>
     <mergeCell ref="V50:AO50"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
@@ -2986,106 +3653,6 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="F14:J14"/>
     <mergeCell ref="A16:L16"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:Q10"/>
-    <mergeCell ref="V1:AO1"/>
-    <mergeCell ref="M31:R31"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="V3:W3"/>
-    <mergeCell ref="X3:Y3"/>
-    <mergeCell ref="X4:Z4"/>
-    <mergeCell ref="Z3:AC3"/>
-    <mergeCell ref="AD3:AG3"/>
-    <mergeCell ref="AH3:AK3"/>
-    <mergeCell ref="K26:R26"/>
-    <mergeCell ref="K27:R27"/>
-    <mergeCell ref="K28:R28"/>
-    <mergeCell ref="H29:L29"/>
-    <mergeCell ref="M30:R30"/>
-    <mergeCell ref="M29:R29"/>
-    <mergeCell ref="K23:R23"/>
-    <mergeCell ref="K24:R24"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="H21:M21"/>
-    <mergeCell ref="H20:M20"/>
-    <mergeCell ref="D15:J15"/>
-    <mergeCell ref="E19:K19"/>
-    <mergeCell ref="E18:K18"/>
-    <mergeCell ref="N11:Q11"/>
-    <mergeCell ref="AC7:AH7"/>
-    <mergeCell ref="Z7:AB7"/>
-    <mergeCell ref="V7:Y7"/>
-    <mergeCell ref="AC8:AH8"/>
-    <mergeCell ref="AC9:AH9"/>
-    <mergeCell ref="AL3:AO3"/>
-    <mergeCell ref="AA4:AC4"/>
-    <mergeCell ref="AD4:AF4"/>
-    <mergeCell ref="AG4:AI4"/>
-    <mergeCell ref="V6:AO6"/>
-    <mergeCell ref="AD11:AG11"/>
-    <mergeCell ref="AD12:AG12"/>
-    <mergeCell ref="AD13:AG13"/>
-    <mergeCell ref="AD14:AG14"/>
-    <mergeCell ref="AD10:AG10"/>
-    <mergeCell ref="V16:AA16"/>
-    <mergeCell ref="V17:AA17"/>
-    <mergeCell ref="V18:AA18"/>
-    <mergeCell ref="V19:AA19"/>
-    <mergeCell ref="AF19:AJ19"/>
-    <mergeCell ref="AF20:AJ20"/>
-    <mergeCell ref="Z23:AB23"/>
-    <mergeCell ref="Z34:AB34"/>
-    <mergeCell ref="V22:Y22"/>
-    <mergeCell ref="V33:Y33"/>
-    <mergeCell ref="AC23:AD23"/>
-    <mergeCell ref="AC15:AD15"/>
-    <mergeCell ref="AC16:AE16"/>
-    <mergeCell ref="AC17:AE17"/>
-    <mergeCell ref="AC18:AE18"/>
-    <mergeCell ref="AC19:AE19"/>
-    <mergeCell ref="AC20:AE20"/>
-    <mergeCell ref="AE15:AJ15"/>
-    <mergeCell ref="AF16:AJ16"/>
-    <mergeCell ref="AF17:AJ17"/>
-    <mergeCell ref="AF18:AJ18"/>
-    <mergeCell ref="V20:AA20"/>
-    <mergeCell ref="V45:Y45"/>
-    <mergeCell ref="V48:Y48"/>
-    <mergeCell ref="Z45:AA45"/>
-    <mergeCell ref="Z48:AA48"/>
-    <mergeCell ref="Z31:AB31"/>
-    <mergeCell ref="AG24:AI24"/>
-    <mergeCell ref="AE27:AL27"/>
-    <mergeCell ref="AG26:AJ26"/>
-    <mergeCell ref="AC34:AD34"/>
-    <mergeCell ref="AE34:AJ34"/>
-    <mergeCell ref="Z22:AJ22"/>
-    <mergeCell ref="Z33:AJ33"/>
-    <mergeCell ref="Z30:AD30"/>
-    <mergeCell ref="AC29:AE29"/>
-    <mergeCell ref="AC27:AD27"/>
-    <mergeCell ref="AC24:AF24"/>
-    <mergeCell ref="AE23:AJ23"/>
-    <mergeCell ref="AC25:AJ25"/>
-    <mergeCell ref="AC28:AG28"/>
-    <mergeCell ref="AH39:AL39"/>
-    <mergeCell ref="AH40:AJ40"/>
-    <mergeCell ref="Z42:AB42"/>
-    <mergeCell ref="AE41:AG41"/>
-    <mergeCell ref="AC41:AD41"/>
-    <mergeCell ref="AC39:AG39"/>
-    <mergeCell ref="AC35:AF35"/>
-    <mergeCell ref="AG35:AI35"/>
-    <mergeCell ref="AC36:AJ36"/>
-    <mergeCell ref="AG37:AJ37"/>
-    <mergeCell ref="AC38:AD38"/>
-    <mergeCell ref="AE38:AL38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4791,6 +5358,786 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC2516D-C382-4EEE-AAC2-D26752816E59}">
+  <dimension ref="A1:L31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>411</v>
+      </c>
+      <c r="B1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C1" t="s">
+        <v>424</v>
+      </c>
+      <c r="D1" t="s">
+        <v>425</v>
+      </c>
+      <c r="E1" t="s">
+        <v>426</v>
+      </c>
+      <c r="G1" t="s">
+        <v>430</v>
+      </c>
+      <c r="I1" t="s">
+        <v>435</v>
+      </c>
+      <c r="J1" t="s">
+        <v>439</v>
+      </c>
+      <c r="L1" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E2" t="s">
+        <v>420</v>
+      </c>
+      <c r="G2" t="s">
+        <v>432</v>
+      </c>
+      <c r="I2" t="s">
+        <v>185</v>
+      </c>
+      <c r="J2" t="s">
+        <v>440</v>
+      </c>
+      <c r="L2" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B3" t="s">
+        <v>419</v>
+      </c>
+      <c r="C3" t="s">
+        <v>427</v>
+      </c>
+      <c r="D3" t="s">
+        <v>428</v>
+      </c>
+      <c r="E3" t="s">
+        <v>429</v>
+      </c>
+      <c r="G3" t="s">
+        <v>431</v>
+      </c>
+      <c r="I3" t="s">
+        <v>437</v>
+      </c>
+      <c r="J3" t="s">
+        <v>441</v>
+      </c>
+      <c r="L3" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>414</v>
+      </c>
+      <c r="B4" t="s">
+        <v>429</v>
+      </c>
+      <c r="C4" t="s">
+        <v>417</v>
+      </c>
+      <c r="D4" t="s">
+        <v>427</v>
+      </c>
+      <c r="E4" t="s">
+        <v>428</v>
+      </c>
+      <c r="G4" t="s">
+        <v>434</v>
+      </c>
+      <c r="I4" t="s">
+        <v>186</v>
+      </c>
+      <c r="J4" t="s">
+        <v>183</v>
+      </c>
+      <c r="L4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>415</v>
+      </c>
+      <c r="B5" t="s">
+        <v>427</v>
+      </c>
+      <c r="C5" t="s">
+        <v>419</v>
+      </c>
+      <c r="D5" t="s">
+        <v>429</v>
+      </c>
+      <c r="E5" t="s">
+        <v>417</v>
+      </c>
+      <c r="G5" t="s">
+        <v>433</v>
+      </c>
+      <c r="I5" t="s">
+        <v>436</v>
+      </c>
+      <c r="J5" t="s">
+        <v>442</v>
+      </c>
+      <c r="L5" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>416</v>
+      </c>
+      <c r="B6" t="s">
+        <v>428</v>
+      </c>
+      <c r="C6" t="s">
+        <v>429</v>
+      </c>
+      <c r="D6" t="s">
+        <v>417</v>
+      </c>
+      <c r="E6" t="s">
+        <v>419</v>
+      </c>
+      <c r="I6" t="s">
+        <v>187</v>
+      </c>
+      <c r="J6" t="s">
+        <v>443</v>
+      </c>
+      <c r="L6" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="I7" t="s">
+        <v>438</v>
+      </c>
+      <c r="L7" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>377</v>
+      </c>
+      <c r="B9" t="s">
+        <v>551</v>
+      </c>
+      <c r="C9" t="s">
+        <v>552</v>
+      </c>
+      <c r="D9" t="s">
+        <v>554</v>
+      </c>
+      <c r="E9" t="s">
+        <v>553</v>
+      </c>
+      <c r="F9" t="s">
+        <v>555</v>
+      </c>
+      <c r="G9" t="s">
+        <v>556</v>
+      </c>
+      <c r="H9" t="s">
+        <v>557</v>
+      </c>
+      <c r="L9" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>558</v>
+      </c>
+      <c r="C10" t="s">
+        <v>559</v>
+      </c>
+      <c r="D10" t="s">
+        <v>560</v>
+      </c>
+      <c r="E10" t="s">
+        <v>561</v>
+      </c>
+      <c r="F10" t="s">
+        <v>562</v>
+      </c>
+      <c r="G10" t="s">
+        <v>563</v>
+      </c>
+      <c r="H10" t="s">
+        <v>564</v>
+      </c>
+      <c r="L10" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>452</v>
+      </c>
+      <c r="B12" t="s">
+        <v>391</v>
+      </c>
+      <c r="C12" t="s">
+        <v>392</v>
+      </c>
+      <c r="D12" t="s">
+        <v>393</v>
+      </c>
+      <c r="E12" t="s">
+        <v>494</v>
+      </c>
+      <c r="F12" t="s">
+        <v>495</v>
+      </c>
+      <c r="G12" t="s">
+        <v>496</v>
+      </c>
+      <c r="H12" t="s">
+        <v>497</v>
+      </c>
+      <c r="I12" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>390</v>
+      </c>
+      <c r="B13" t="s">
+        <v>394</v>
+      </c>
+      <c r="C13" t="s">
+        <v>396</v>
+      </c>
+      <c r="D13" t="s">
+        <v>397</v>
+      </c>
+      <c r="E13" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>395</v>
+      </c>
+      <c r="C14" t="s">
+        <v>398</v>
+      </c>
+      <c r="D14" t="s">
+        <v>400</v>
+      </c>
+      <c r="E14" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>399</v>
+      </c>
+      <c r="E15" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>449</v>
+      </c>
+      <c r="B17" t="s">
+        <v>453</v>
+      </c>
+      <c r="C17" t="s">
+        <v>454</v>
+      </c>
+      <c r="D17" t="s">
+        <v>455</v>
+      </c>
+      <c r="E17" t="s">
+        <v>456</v>
+      </c>
+      <c r="F17" t="s">
+        <v>457</v>
+      </c>
+      <c r="I17" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>450</v>
+      </c>
+      <c r="B22" t="s">
+        <v>378</v>
+      </c>
+      <c r="C22" t="s">
+        <v>463</v>
+      </c>
+      <c r="D22" t="s">
+        <v>464</v>
+      </c>
+      <c r="E22" t="s">
+        <v>461</v>
+      </c>
+      <c r="F22" t="s">
+        <v>465</v>
+      </c>
+      <c r="G22" t="s">
+        <v>462</v>
+      </c>
+      <c r="H22" t="s">
+        <v>467</v>
+      </c>
+      <c r="I22" t="s">
+        <v>466</v>
+      </c>
+      <c r="J22" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>379</v>
+      </c>
+      <c r="B23" t="s">
+        <v>380</v>
+      </c>
+      <c r="C23" t="s">
+        <v>382</v>
+      </c>
+      <c r="D23" t="s">
+        <v>383</v>
+      </c>
+      <c r="E23" t="s">
+        <v>384</v>
+      </c>
+      <c r="F23" t="s">
+        <v>385</v>
+      </c>
+      <c r="G23" t="s">
+        <v>386</v>
+      </c>
+      <c r="H23" t="s">
+        <v>388</v>
+      </c>
+      <c r="I23" t="s">
+        <v>421</v>
+      </c>
+      <c r="J23" t="s">
+        <v>444</v>
+      </c>
+      <c r="K23" t="s">
+        <v>446</v>
+      </c>
+      <c r="L23" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>381</v>
+      </c>
+      <c r="G24" t="s">
+        <v>387</v>
+      </c>
+      <c r="H24" t="s">
+        <v>389</v>
+      </c>
+      <c r="I24" t="s">
+        <v>422</v>
+      </c>
+      <c r="J24" t="s">
+        <v>445</v>
+      </c>
+      <c r="K24" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>451</v>
+      </c>
+      <c r="B26" t="s">
+        <v>404</v>
+      </c>
+      <c r="C26" t="s">
+        <v>486</v>
+      </c>
+      <c r="D26" t="s">
+        <v>487</v>
+      </c>
+      <c r="E26" t="s">
+        <v>488</v>
+      </c>
+      <c r="F26" t="s">
+        <v>489</v>
+      </c>
+      <c r="G26" t="s">
+        <v>491</v>
+      </c>
+      <c r="H26" t="s">
+        <v>492</v>
+      </c>
+      <c r="I26" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>410</v>
+      </c>
+      <c r="B27" t="s">
+        <v>405</v>
+      </c>
+      <c r="C27" t="s">
+        <v>406</v>
+      </c>
+      <c r="D27" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>409</v>
+      </c>
+      <c r="D28" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>459</v>
+      </c>
+      <c r="B30" t="s">
+        <v>479</v>
+      </c>
+      <c r="C30" t="s">
+        <v>480</v>
+      </c>
+      <c r="D30" t="s">
+        <v>481</v>
+      </c>
+      <c r="E30" t="s">
+        <v>482</v>
+      </c>
+      <c r="F30" t="s">
+        <v>483</v>
+      </c>
+      <c r="G30" t="s">
+        <v>484</v>
+      </c>
+      <c r="H30" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>460</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CBE5ED5-CE79-40AD-98B6-C605BB8571E8}">
+  <dimension ref="D1:F16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>535</v>
+      </c>
+      <c r="F1" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="2" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>536</v>
+      </c>
+      <c r="F2" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="3" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D3" t="s">
+        <v>537</v>
+      </c>
+      <c r="F3" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="4" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>538</v>
+      </c>
+      <c r="F4" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="5" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>539</v>
+      </c>
+      <c r="F5" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>540</v>
+      </c>
+      <c r="F6" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="7" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>541</v>
+      </c>
+      <c r="F7" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="8" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>542</v>
+      </c>
+      <c r="F8" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="9" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>543</v>
+      </c>
+      <c r="F9" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="10" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D10" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="11" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="12" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="13" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="14" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D14" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="15" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D15" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="16" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D16" t="s">
+        <v>550</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71282E59-1908-45D6-8F2B-7B94D73F4D27}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>508</v>
+      </c>
+      <c r="C1" t="s">
+        <v>512</v>
+      </c>
+      <c r="D1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>509</v>
+      </c>
+      <c r="C2" t="s">
+        <v>513</v>
+      </c>
+      <c r="D2" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>510</v>
+      </c>
+      <c r="C3" t="s">
+        <v>514</v>
+      </c>
+      <c r="D3" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>511</v>
+      </c>
+      <c r="C4" t="s">
+        <v>515</v>
+      </c>
+      <c r="D4" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>516</v>
+      </c>
+      <c r="D5" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>517</v>
+      </c>
+      <c r="D6" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>518</v>
+      </c>
+      <c r="D7" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>519</v>
+      </c>
+      <c r="D8" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>520</v>
+      </c>
+      <c r="D9" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>521</v>
+      </c>
+      <c r="D10" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D11" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D12" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
+        <v>534</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD3BA5F0-F4D6-42DF-955B-2C6E884E8104}">
   <dimension ref="A1:A8"/>
   <sheetViews>

</xml_diff>